<commit_message>
Updated asset list, added character and scene list.
</commit_message>
<xml_diff>
--- a/Doorman_Documents/Asset List.xlsx
+++ b/Doorman_Documents/Asset List.xlsx
@@ -19,14 +19,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="74">
   <si>
     <t>Type</t>
   </si>
   <si>
-    <t>Name</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
@@ -48,9 +45,6 @@
     <t>Bg_Buttons.jpg</t>
   </si>
   <si>
-    <t xml:space="preserve">elevator buttons </t>
-  </si>
-  <si>
     <t>Not Done</t>
   </si>
   <si>
@@ -63,9 +57,6 @@
     <t>sound</t>
   </si>
   <si>
-    <t>scene</t>
-  </si>
-  <si>
     <t>Specs</t>
   </si>
   <si>
@@ -76,6 +67,180 @@
   </si>
   <si>
     <t>Placeholder</t>
+  </si>
+  <si>
+    <t>File Name</t>
+  </si>
+  <si>
+    <t>Bg_Lobby.jpg</t>
+  </si>
+  <si>
+    <t>Hotel lobby and conversation hub</t>
+  </si>
+  <si>
+    <t>Bg_Lobbyblur.jpg</t>
+  </si>
+  <si>
+    <t>Blurred lobby image during dialogue</t>
+  </si>
+  <si>
+    <t>Bg_Elevator.jpg</t>
+  </si>
+  <si>
+    <t>Elevator scene to choose floors</t>
+  </si>
+  <si>
+    <t>Elevator zoomed in to choose floors</t>
+  </si>
+  <si>
+    <t>Bg_Hall.jpg</t>
+  </si>
+  <si>
+    <t>Hotel floor hallway to choose room</t>
+  </si>
+  <si>
+    <t>Bg_Room.jpg</t>
+  </si>
+  <si>
+    <t>Hotel room to select hiding place</t>
+  </si>
+  <si>
+    <t>Bg_Jimroom.jpg</t>
+  </si>
+  <si>
+    <t>Jim's room at the start of the game</t>
+  </si>
+  <si>
+    <t>Bg_Jail.jpg</t>
+  </si>
+  <si>
+    <t>Jail cell, lose state of the game</t>
+  </si>
+  <si>
+    <t>Bg_Shop.jpg</t>
+  </si>
+  <si>
+    <t>Pawn shop win state of the game</t>
+  </si>
+  <si>
+    <t>Char_Chris.png</t>
+  </si>
+  <si>
+    <t>Character image of Chris</t>
+  </si>
+  <si>
+    <t>847 X 1080</t>
+  </si>
+  <si>
+    <t>Char_Coach.png</t>
+  </si>
+  <si>
+    <t>Character image of Coach Dave</t>
+  </si>
+  <si>
+    <t>Char_Colonel.png</t>
+  </si>
+  <si>
+    <t>Character image of Colonel Ketchup</t>
+  </si>
+  <si>
+    <t>Char_Edmond.png</t>
+  </si>
+  <si>
+    <t>Character image of Sir Edmond</t>
+  </si>
+  <si>
+    <t>Char_Jason.png</t>
+  </si>
+  <si>
+    <t>Character image of Jason</t>
+  </si>
+  <si>
+    <t>Char_Kim.png</t>
+  </si>
+  <si>
+    <t>Character image of Kim</t>
+  </si>
+  <si>
+    <t>Char_Madam.png</t>
+  </si>
+  <si>
+    <t>Character image of Madam Feline</t>
+  </si>
+  <si>
+    <t>Doorman_Logo.png</t>
+  </si>
+  <si>
+    <t>Logo of the game</t>
+  </si>
+  <si>
+    <t>1920 X 636</t>
+  </si>
+  <si>
+    <t>Finished</t>
+  </si>
+  <si>
+    <t>Doorman_Icon.png</t>
+  </si>
+  <si>
+    <t>Desktop icon for the game exec.</t>
+  </si>
+  <si>
+    <t>478 X 479</t>
+  </si>
+  <si>
+    <t>Main menu screen</t>
+  </si>
+  <si>
+    <t>Bg_Menu.jpg</t>
+  </si>
+  <si>
+    <t>Bg_Options.jpg</t>
+  </si>
+  <si>
+    <t>Options screen</t>
+  </si>
+  <si>
+    <t>Bg_Difficulty.jpg</t>
+  </si>
+  <si>
+    <t>Difficulty select screen</t>
+  </si>
+  <si>
+    <t>Bg_Gmenu.jpg</t>
+  </si>
+  <si>
+    <t>In-game menu screen</t>
+  </si>
+  <si>
+    <t>Bg_Credits.jpg</t>
+  </si>
+  <si>
+    <t>Credits screen</t>
+  </si>
+  <si>
+    <t>Background music for menu</t>
+  </si>
+  <si>
+    <t>Background music for lobby</t>
+  </si>
+  <si>
+    <t>Background music for night-time</t>
+  </si>
+  <si>
+    <t>Elevator beeping sound to signal floor select.</t>
+  </si>
+  <si>
+    <t>Music/sound for lose state</t>
+  </si>
+  <si>
+    <t>Music/sound for win state</t>
+  </si>
+  <si>
+    <t>Sound for pressing a menu/dialogue button</t>
+  </si>
+  <si>
+    <t>Sound for a character leaving a scene (door sound)</t>
   </si>
 </sst>
 </file>
@@ -406,7 +571,7 @@
   <dimension ref="A1:AC50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -421,25 +586,25 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
       </c>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
@@ -465,352 +630,674 @@
     </row>
     <row r="2" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="H2" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
+      <c r="E3" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="F3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" s="4"/>
+        <v>15</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="4" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="F4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" s="4"/>
+        <v>15</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="5" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
+      <c r="A5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="F5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" s="4"/>
+        <v>15</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="6" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
+      <c r="A6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="F6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6" s="4"/>
+        <v>15</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="7" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
+      <c r="A7" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="F7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G7" s="4"/>
+        <v>15</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="8" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D8" s="4"/>
+      <c r="A8" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>13</v>
+      </c>
       <c r="E8" s="4"/>
       <c r="F8" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G8" s="4"/>
     </row>
     <row r="9" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D9" s="4"/>
+      <c r="A9" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>13</v>
+      </c>
       <c r="E9" s="4"/>
       <c r="F9" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G9" s="4"/>
     </row>
     <row r="10" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D10" s="4"/>
+      <c r="A10" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>13</v>
+      </c>
       <c r="E10" s="4"/>
       <c r="F10" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G10" s="4"/>
     </row>
     <row r="11" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
+      <c r="A11" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="F11" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="G11" s="4"/>
     </row>
     <row r="12" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
+      <c r="A12" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="F12" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="G12" s="4"/>
     </row>
     <row r="13" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
+      <c r="A13" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="F13" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="G13" s="4"/>
     </row>
     <row r="14" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
+      <c r="A14" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="F14" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="G14" s="4"/>
     </row>
     <row r="15" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
+      <c r="A15" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" t="s">
+        <v>44</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="F15" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="G15" s="4"/>
     </row>
     <row r="16" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
+      <c r="A16" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" t="s">
+        <v>46</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="F16" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="G16" s="4"/>
     </row>
-    <row r="17" spans="4:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
+    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="F17" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="G17" s="4"/>
     </row>
-    <row r="18" spans="4:7" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
+    <row r="18" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18" t="s">
+        <v>50</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="F18" s="1" t="s">
-        <v>10</v>
+        <v>52</v>
       </c>
       <c r="G18" s="4"/>
     </row>
-    <row r="19" spans="4:7" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
+    <row r="19" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19" t="s">
+        <v>54</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="F19" s="1" t="s">
-        <v>10</v>
+        <v>52</v>
       </c>
       <c r="G19" s="4"/>
     </row>
-    <row r="20" spans="4:7" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="D20" s="4"/>
+    <row r="20" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" t="s">
+        <v>57</v>
+      </c>
+      <c r="C20" t="s">
+        <v>56</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>13</v>
+      </c>
       <c r="E20" s="4"/>
       <c r="F20" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G20" s="4"/>
     </row>
-    <row r="21" spans="4:7" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="D21" s="4"/>
+    <row r="21" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" t="s">
+        <v>58</v>
+      </c>
+      <c r="C21" t="s">
+        <v>59</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>13</v>
+      </c>
       <c r="E21" s="4"/>
       <c r="F21" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G21" s="4"/>
     </row>
-    <row r="22" spans="4:7" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="D22" s="4"/>
+    <row r="22" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" t="s">
+        <v>60</v>
+      </c>
+      <c r="C22" t="s">
+        <v>61</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>13</v>
+      </c>
       <c r="E22" s="4"/>
       <c r="F22" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G22" s="4"/>
     </row>
-    <row r="23" spans="4:7" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="D23" s="4"/>
+    <row r="23" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" t="s">
+        <v>62</v>
+      </c>
+      <c r="C23" t="s">
+        <v>63</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>13</v>
+      </c>
       <c r="E23" s="4"/>
       <c r="F23" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G23" s="4"/>
     </row>
-    <row r="24" spans="4:7" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="D24" s="4"/>
+    <row r="24" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" t="s">
+        <v>64</v>
+      </c>
+      <c r="C24" t="s">
+        <v>65</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>13</v>
+      </c>
       <c r="E24" s="4"/>
       <c r="F24" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G24" s="4"/>
     </row>
-    <row r="25" spans="4:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C25" t="s">
+        <v>66</v>
+      </c>
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
       <c r="F25" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G25" s="4"/>
     </row>
-    <row r="26" spans="4:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C26" t="s">
+        <v>67</v>
+      </c>
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
       <c r="F26" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G26" s="4"/>
     </row>
-    <row r="27" spans="4:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C27" t="s">
+        <v>68</v>
+      </c>
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
       <c r="F27" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G27" s="4"/>
     </row>
-    <row r="28" spans="4:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C28" t="s">
+        <v>69</v>
+      </c>
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
       <c r="F28" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G28" s="4"/>
     </row>
-    <row r="29" spans="4:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C29" t="s">
+        <v>70</v>
+      </c>
       <c r="F29" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="30" spans="4:7" ht="13.2" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C30" t="s">
+        <v>71</v>
+      </c>
       <c r="F30" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="31" spans="4:7" ht="13.2" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C31" t="s">
+        <v>72</v>
+      </c>
       <c r="F31" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="32" spans="4:7" ht="13.2" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C32" t="s">
+        <v>73</v>
+      </c>
       <c r="F32" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="33" spans="6:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="F33" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="34" spans="6:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="F34" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="35" spans="6:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="F35" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="36" spans="6:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="F36" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="37" spans="6:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="F37" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="38" spans="6:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="F38" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="39" spans="6:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="F39" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="40" spans="6:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="F40" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="41" spans="6:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="F41" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="42" spans="6:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="F42" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="43" spans="6:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="F43" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="44" spans="6:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="F44" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="45" spans="6:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="F45" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="46" spans="6:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="F46" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="47" spans="6:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="F47" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="48" spans="6:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="F48" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="49" spans="6:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="F49" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="50" spans="6:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="F50" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Jail and Pawn Shop BG's, update Assets list.
</commit_message>
<xml_diff>
--- a/Doorman_Documents/Asset List.xlsx
+++ b/Doorman_Documents/Asset List.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="74">
   <si>
     <t>Type</t>
   </si>
@@ -571,7 +571,7 @@
   <dimension ref="A1:AC50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -801,9 +801,11 @@
       <c r="D9" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="4"/>
+      <c r="E9" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="F9" s="1" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="G9" s="4"/>
     </row>
@@ -820,9 +822,11 @@
       <c r="D10" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="4"/>
+      <c r="E10" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="F10" s="1" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="G10" s="4"/>
     </row>

</xml_diff>

<commit_message>
Added placeholders for intro sequence, update asset list with new image assets needed.
</commit_message>
<xml_diff>
--- a/Doorman_Documents/Asset List.xlsx
+++ b/Doorman_Documents/Asset List.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="94">
   <si>
     <t>Type</t>
   </si>
@@ -241,6 +241,66 @@
   </si>
   <si>
     <t>Sound for a character leaving a scene (door sound)</t>
+  </si>
+  <si>
+    <t>Item_Phone.png</t>
+  </si>
+  <si>
+    <t>Phone item, used in Jim's Room</t>
+  </si>
+  <si>
+    <t>460 X 856</t>
+  </si>
+  <si>
+    <t>Item_Splicer.png</t>
+  </si>
+  <si>
+    <t>DNA Splicer, Madam Feline's item</t>
+  </si>
+  <si>
+    <t>Item_Flour.png</t>
+  </si>
+  <si>
+    <t>Bag of flour, Chris's item</t>
+  </si>
+  <si>
+    <t>Item_Fleece.png</t>
+  </si>
+  <si>
+    <t>Golden fleece blanket, Jason's item</t>
+  </si>
+  <si>
+    <t>Item_Football.png</t>
+  </si>
+  <si>
+    <t>Deflated football, Coach Dave's item</t>
+  </si>
+  <si>
+    <t>Item_Watch.png</t>
+  </si>
+  <si>
+    <t>Diamond Pocket Watch, Sir Edmond's item</t>
+  </si>
+  <si>
+    <t>Item_Heels.png</t>
+  </si>
+  <si>
+    <t>High Heels, Kim's item</t>
+  </si>
+  <si>
+    <t>Item_Candle.png</t>
+  </si>
+  <si>
+    <t>Candlestick, Colonel Ketchup's item</t>
+  </si>
+  <si>
+    <t>Phone ringing</t>
+  </si>
+  <si>
+    <t>Item_Clock.png</t>
+  </si>
+  <si>
+    <t>Clock, shows player how much time they have</t>
   </si>
 </sst>
 </file>
@@ -568,10 +628,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC50"/>
+  <dimension ref="A1:AC59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -782,9 +842,11 @@
       <c r="D8" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="4"/>
+      <c r="E8" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="F8" s="1" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="G8" s="4"/>
     </row>
@@ -977,319 +1039,437 @@
       </c>
       <c r="G17" s="4"/>
     </row>
-    <row r="18" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B18" t="s">
-        <v>49</v>
+        <v>74</v>
       </c>
       <c r="C18" t="s">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>51</v>
+        <v>76</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F18" s="1" t="s">
-        <v>52</v>
+      <c r="F18" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="G18" s="4"/>
     </row>
-    <row r="19" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B19" t="s">
-        <v>53</v>
+        <v>92</v>
       </c>
       <c r="C19" t="s">
-        <v>54</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>52</v>
+        <v>93</v>
+      </c>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="G19" s="4"/>
     </row>
-    <row r="20" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B20" t="s">
-        <v>57</v>
+        <v>77</v>
       </c>
       <c r="C20" t="s">
-        <v>56</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>13</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="D20" s="4"/>
       <c r="E20" s="4"/>
-      <c r="F20" s="1" t="s">
+      <c r="F20" s="2" t="s">
         <v>8</v>
       </c>
       <c r="G20" s="4"/>
     </row>
-    <row r="21" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B21" t="s">
-        <v>58</v>
+        <v>79</v>
       </c>
       <c r="C21" t="s">
-        <v>59</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>13</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="D21" s="4"/>
       <c r="E21" s="4"/>
-      <c r="F21" s="1" t="s">
+      <c r="F21" s="2" t="s">
         <v>8</v>
       </c>
       <c r="G21" s="4"/>
     </row>
-    <row r="22" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B22" t="s">
-        <v>60</v>
+        <v>81</v>
       </c>
       <c r="C22" t="s">
-        <v>61</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>13</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="D22" s="4"/>
       <c r="E22" s="4"/>
-      <c r="F22" s="1" t="s">
+      <c r="F22" s="2" t="s">
         <v>8</v>
       </c>
       <c r="G22" s="4"/>
     </row>
-    <row r="23" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B23" t="s">
-        <v>62</v>
+        <v>83</v>
       </c>
       <c r="C23" t="s">
-        <v>63</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>13</v>
-      </c>
+        <v>84</v>
+      </c>
+      <c r="D23" s="4"/>
       <c r="E23" s="4"/>
-      <c r="F23" s="1" t="s">
+      <c r="F23" s="2" t="s">
         <v>8</v>
       </c>
       <c r="G23" s="4"/>
     </row>
-    <row r="24" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B24" t="s">
-        <v>64</v>
+        <v>85</v>
       </c>
       <c r="C24" t="s">
-        <v>65</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>13</v>
-      </c>
+        <v>86</v>
+      </c>
+      <c r="D24" s="4"/>
       <c r="E24" s="4"/>
-      <c r="F24" s="1" t="s">
+      <c r="F24" s="2" t="s">
         <v>8</v>
       </c>
       <c r="G24" s="4"/>
     </row>
-    <row r="25" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>11</v>
+        <v>6</v>
+      </c>
+      <c r="B25" t="s">
+        <v>87</v>
       </c>
       <c r="C25" t="s">
-        <v>66</v>
+        <v>88</v>
       </c>
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
-      <c r="F25" s="1" t="s">
+      <c r="F25" s="2" t="s">
         <v>8</v>
       </c>
       <c r="G25" s="4"/>
     </row>
-    <row r="26" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>11</v>
+        <v>6</v>
+      </c>
+      <c r="B26" t="s">
+        <v>89</v>
       </c>
       <c r="C26" t="s">
-        <v>67</v>
+        <v>90</v>
       </c>
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
-      <c r="F26" s="1" t="s">
+      <c r="F26" s="2" t="s">
         <v>8</v>
       </c>
       <c r="G26" s="4"/>
     </row>
     <row r="27" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>11</v>
+        <v>6</v>
+      </c>
+      <c r="B27" t="s">
+        <v>49</v>
       </c>
       <c r="C27" t="s">
-        <v>68</v>
-      </c>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
+        <v>50</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="F27" s="1" t="s">
-        <v>8</v>
+        <v>52</v>
       </c>
       <c r="G27" s="4"/>
     </row>
     <row r="28" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>11</v>
+        <v>6</v>
+      </c>
+      <c r="B28" t="s">
+        <v>53</v>
       </c>
       <c r="C28" t="s">
-        <v>69</v>
-      </c>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
+        <v>54</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="F28" s="1" t="s">
-        <v>8</v>
+        <v>52</v>
       </c>
       <c r="G28" s="4"/>
     </row>
     <row r="29" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>11</v>
+        <v>6</v>
+      </c>
+      <c r="B29" t="s">
+        <v>57</v>
       </c>
       <c r="C29" t="s">
-        <v>70</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E29" s="4"/>
       <c r="F29" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="G29" s="4"/>
     </row>
     <row r="30" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>11</v>
+        <v>6</v>
+      </c>
+      <c r="B30" t="s">
+        <v>58</v>
       </c>
       <c r="C30" t="s">
-        <v>71</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E30" s="4"/>
       <c r="F30" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="G30" s="4"/>
     </row>
     <row r="31" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>11</v>
+        <v>6</v>
+      </c>
+      <c r="B31" t="s">
+        <v>60</v>
       </c>
       <c r="C31" t="s">
-        <v>72</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E31" s="4"/>
       <c r="F31" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="G31" s="4"/>
     </row>
     <row r="32" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B32" t="s">
+        <v>62</v>
+      </c>
+      <c r="C32" t="s">
+        <v>63</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E32" s="4"/>
+      <c r="F32" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G32" s="4"/>
+    </row>
+    <row r="33" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33" t="s">
+        <v>64</v>
+      </c>
+      <c r="C33" t="s">
+        <v>65</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E33" s="4"/>
+      <c r="F33" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G33" s="4"/>
+    </row>
+    <row r="34" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C34" t="s">
+        <v>66</v>
+      </c>
+      <c r="D34" s="4"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G34" s="4"/>
+    </row>
+    <row r="35" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C35" t="s">
+        <v>67</v>
+      </c>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G35" s="4"/>
+    </row>
+    <row r="36" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A36" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C36" t="s">
+        <v>68</v>
+      </c>
+      <c r="D36" s="4"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G36" s="4"/>
+    </row>
+    <row r="37" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C37" t="s">
+        <v>69</v>
+      </c>
+      <c r="D37" s="4"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G37" s="4"/>
+    </row>
+    <row r="38" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C38" t="s">
+        <v>70</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A39" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C39" t="s">
+        <v>71</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C40" t="s">
+        <v>72</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A41" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C41" t="s">
         <v>73</v>
       </c>
-      <c r="F32" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="33" spans="6:6" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="F33" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="34" spans="6:6" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="F34" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="35" spans="6:6" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="F35" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="36" spans="6:6" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="F36" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="37" spans="6:6" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="F37" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="38" spans="6:6" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="F38" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="39" spans="6:6" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="F39" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="40" spans="6:6" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="F40" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="41" spans="6:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="F41" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="42" spans="6:6" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A42" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C42" t="s">
+        <v>91</v>
+      </c>
       <c r="F42" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="43" spans="6:6" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="F43" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="44" spans="6:6" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="F44" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="45" spans="6:6" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="F45" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="46" spans="6:6" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="F46" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="47" spans="6:6" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="F47" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="48" spans="6:6" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="F48" s="1" t="s">
         <v>8</v>
       </c>
@@ -1301,6 +1481,51 @@
     </row>
     <row r="50" spans="6:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="F50" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="51" spans="6:6" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F51" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="52" spans="6:6" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F52" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="53" spans="6:6" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F53" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="54" spans="6:6" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F54" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="55" spans="6:6" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F55" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="56" spans="6:6" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F56" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="57" spans="6:6" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F57" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="58" spans="6:6" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F58" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="59" spans="6:6" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F59" s="1" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added assets for all character items, updated asset list.
</commit_message>
<xml_diff>
--- a/Doorman_Documents/Asset List.xlsx
+++ b/Doorman_Documents/Asset List.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="103">
   <si>
     <t>Type</t>
   </si>
@@ -301,6 +301,33 @@
   </si>
   <si>
     <t>Clock, shows player how much time they have</t>
+  </si>
+  <si>
+    <t>499 X 793</t>
+  </si>
+  <si>
+    <t>750 X 711</t>
+  </si>
+  <si>
+    <t>563 X 606</t>
+  </si>
+  <si>
+    <t>793 X 568</t>
+  </si>
+  <si>
+    <t>501 X 613</t>
+  </si>
+  <si>
+    <t>596 X 682</t>
+  </si>
+  <si>
+    <t>588 X 615</t>
+  </si>
+  <si>
+    <t>Item_Clock_Cycle.png</t>
+  </si>
+  <si>
+    <t>Sprite sheet for the time that has passed</t>
   </si>
 </sst>
 </file>
@@ -628,10 +655,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC59"/>
+  <dimension ref="A1:AC60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1082,10 +1109,10 @@
         <v>6</v>
       </c>
       <c r="B20" t="s">
-        <v>77</v>
+        <v>101</v>
       </c>
       <c r="C20" t="s">
-        <v>78</v>
+        <v>102</v>
       </c>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
@@ -1099,15 +1126,19 @@
         <v>6</v>
       </c>
       <c r="B21" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C21" t="s">
-        <v>80</v>
-      </c>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
+        <v>78</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="F21" s="2" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="G21" s="4"/>
     </row>
@@ -1116,15 +1147,19 @@
         <v>6</v>
       </c>
       <c r="B22" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C22" t="s">
-        <v>82</v>
-      </c>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
+        <v>80</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="F22" s="2" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="G22" s="4"/>
     </row>
@@ -1133,15 +1168,19 @@
         <v>6</v>
       </c>
       <c r="B23" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C23" t="s">
-        <v>84</v>
-      </c>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
+        <v>82</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="F23" s="2" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="G23" s="4"/>
     </row>
@@ -1150,15 +1189,19 @@
         <v>6</v>
       </c>
       <c r="B24" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C24" t="s">
-        <v>86</v>
-      </c>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
+        <v>84</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="F24" s="2" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="G24" s="4"/>
     </row>
@@ -1167,15 +1210,19 @@
         <v>6</v>
       </c>
       <c r="B25" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C25" t="s">
-        <v>88</v>
-      </c>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
+        <v>86</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="F25" s="2" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="G25" s="4"/>
     </row>
@@ -1184,36 +1231,40 @@
         <v>6</v>
       </c>
       <c r="B26" t="s">
+        <v>87</v>
+      </c>
+      <c r="C26" t="s">
+        <v>88</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G26" s="4"/>
+    </row>
+    <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27" t="s">
         <v>89</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C27" t="s">
         <v>90</v>
       </c>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G26" s="4"/>
-    </row>
-    <row r="27" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B27" t="s">
-        <v>49</v>
-      </c>
-      <c r="C27" t="s">
-        <v>50</v>
-      </c>
       <c r="D27" s="4" t="s">
-        <v>51</v>
+        <v>100</v>
       </c>
       <c r="E27" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F27" s="1" t="s">
-        <v>52</v>
+      <c r="F27" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="G27" s="4"/>
     </row>
@@ -1222,13 +1273,13 @@
         <v>6</v>
       </c>
       <c r="B28" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C28" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E28" s="4" t="s">
         <v>14</v>
@@ -1243,17 +1294,19 @@
         <v>6</v>
       </c>
       <c r="B29" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C29" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E29" s="4"/>
+        <v>55</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="F29" s="1" t="s">
-        <v>8</v>
+        <v>52</v>
       </c>
       <c r="G29" s="4"/>
     </row>
@@ -1262,10 +1315,10 @@
         <v>6</v>
       </c>
       <c r="B30" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C30" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D30" s="4" t="s">
         <v>13</v>
@@ -1281,10 +1334,10 @@
         <v>6</v>
       </c>
       <c r="B31" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C31" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D31" s="4" t="s">
         <v>13</v>
@@ -1300,10 +1353,10 @@
         <v>6</v>
       </c>
       <c r="B32" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C32" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D32" s="4" t="s">
         <v>13</v>
@@ -1319,10 +1372,10 @@
         <v>6</v>
       </c>
       <c r="B33" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C33" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D33" s="4" t="s">
         <v>13</v>
@@ -1335,12 +1388,17 @@
     </row>
     <row r="34" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>11</v>
+        <v>6</v>
+      </c>
+      <c r="B34" t="s">
+        <v>64</v>
       </c>
       <c r="C34" t="s">
-        <v>66</v>
-      </c>
-      <c r="D34" s="4"/>
+        <v>65</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>13</v>
+      </c>
       <c r="E34" s="4"/>
       <c r="F34" s="1" t="s">
         <v>8</v>
@@ -1352,7 +1410,7 @@
         <v>11</v>
       </c>
       <c r="C35" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D35" s="4"/>
       <c r="E35" s="4"/>
@@ -1366,7 +1424,7 @@
         <v>11</v>
       </c>
       <c r="C36" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D36" s="4"/>
       <c r="E36" s="4"/>
@@ -1380,7 +1438,7 @@
         <v>11</v>
       </c>
       <c r="C37" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D37" s="4"/>
       <c r="E37" s="4"/>
@@ -1394,18 +1452,21 @@
         <v>11</v>
       </c>
       <c r="C38" t="s">
-        <v>70</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="D38" s="4"/>
+      <c r="E38" s="4"/>
       <c r="F38" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="G38" s="4"/>
     </row>
     <row r="39" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C39" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F39" s="1" t="s">
         <v>8</v>
@@ -1416,7 +1477,7 @@
         <v>11</v>
       </c>
       <c r="C40" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F40" s="1" t="s">
         <v>8</v>
@@ -1427,7 +1488,7 @@
         <v>11</v>
       </c>
       <c r="C41" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F41" s="1" t="s">
         <v>8</v>
@@ -1438,13 +1499,19 @@
         <v>11</v>
       </c>
       <c r="C42" t="s">
+        <v>73</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A43" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C43" t="s">
         <v>91</v>
       </c>
-      <c r="F42" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="F43" s="1" t="s">
         <v>8</v>
       </c>
@@ -1526,6 +1593,11 @@
     </row>
     <row r="59" spans="6:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="F59" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="60" spans="6:6" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F60" s="1" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated game script with all completed images, duped images folder into game folder so images would work, added opening scene.
</commit_message>
<xml_diff>
--- a/Doorman_Documents/Asset List.xlsx
+++ b/Doorman_Documents/Asset List.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="106">
   <si>
     <t>Type</t>
   </si>
@@ -324,10 +324,19 @@
     <t>588 X 615</t>
   </si>
   <si>
-    <t>Item_Clock_Cycle.png</t>
-  </si>
-  <si>
-    <t>Sprite sheet for the time that has passed</t>
+    <t>297 X 297</t>
+  </si>
+  <si>
+    <t>Item_Clock_Minute.png</t>
+  </si>
+  <si>
+    <t>Minute hand for the clock</t>
+  </si>
+  <si>
+    <t>Item_Clock_Hour.png</t>
+  </si>
+  <si>
+    <t>Hour hand for the clock</t>
   </si>
 </sst>
 </file>
@@ -655,10 +664,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC60"/>
+  <dimension ref="A1:AC61"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1097,10 +1106,14 @@
       <c r="C19" t="s">
         <v>93</v>
       </c>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
+      <c r="D19" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="F19" s="2" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="G19" s="4"/>
     </row>
@@ -1109,15 +1122,19 @@
         <v>6</v>
       </c>
       <c r="B20" t="s">
+        <v>102</v>
+      </c>
+      <c r="C20" t="s">
+        <v>103</v>
+      </c>
+      <c r="D20" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="C20" t="s">
-        <v>102</v>
-      </c>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
+      <c r="E20" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="F20" s="2" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="G20" s="4"/>
     </row>
@@ -1126,13 +1143,13 @@
         <v>6</v>
       </c>
       <c r="B21" t="s">
-        <v>77</v>
+        <v>104</v>
       </c>
       <c r="C21" t="s">
-        <v>78</v>
+        <v>105</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="E21" s="4" t="s">
         <v>14</v>
@@ -1147,13 +1164,13 @@
         <v>6</v>
       </c>
       <c r="B22" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C22" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E22" s="4" t="s">
         <v>14</v>
@@ -1168,13 +1185,13 @@
         <v>6</v>
       </c>
       <c r="B23" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C23" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E23" s="4" t="s">
         <v>14</v>
@@ -1189,13 +1206,13 @@
         <v>6</v>
       </c>
       <c r="B24" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C24" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E24" s="4" t="s">
         <v>14</v>
@@ -1210,13 +1227,13 @@
         <v>6</v>
       </c>
       <c r="B25" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C25" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E25" s="4" t="s">
         <v>14</v>
@@ -1231,13 +1248,13 @@
         <v>6</v>
       </c>
       <c r="B26" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C26" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E26" s="4" t="s">
         <v>14</v>
@@ -1252,40 +1269,40 @@
         <v>6</v>
       </c>
       <c r="B27" t="s">
+        <v>87</v>
+      </c>
+      <c r="C27" t="s">
+        <v>88</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G27" s="4"/>
+    </row>
+    <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28" t="s">
         <v>89</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C28" t="s">
         <v>90</v>
       </c>
-      <c r="D27" s="4" t="s">
+      <c r="D28" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="E27" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G27" s="4"/>
-    </row>
-    <row r="28" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B28" t="s">
-        <v>49</v>
-      </c>
-      <c r="C28" t="s">
-        <v>50</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>51</v>
-      </c>
       <c r="E28" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F28" s="1" t="s">
-        <v>52</v>
+      <c r="F28" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="G28" s="4"/>
     </row>
@@ -1294,13 +1311,13 @@
         <v>6</v>
       </c>
       <c r="B29" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C29" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E29" s="4" t="s">
         <v>14</v>
@@ -1315,17 +1332,19 @@
         <v>6</v>
       </c>
       <c r="B30" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C30" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E30" s="4"/>
+        <v>55</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="F30" s="1" t="s">
-        <v>8</v>
+        <v>52</v>
       </c>
       <c r="G30" s="4"/>
     </row>
@@ -1334,10 +1353,10 @@
         <v>6</v>
       </c>
       <c r="B31" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C31" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D31" s="4" t="s">
         <v>13</v>
@@ -1353,10 +1372,10 @@
         <v>6</v>
       </c>
       <c r="B32" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C32" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D32" s="4" t="s">
         <v>13</v>
@@ -1372,10 +1391,10 @@
         <v>6</v>
       </c>
       <c r="B33" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C33" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D33" s="4" t="s">
         <v>13</v>
@@ -1391,10 +1410,10 @@
         <v>6</v>
       </c>
       <c r="B34" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C34" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D34" s="4" t="s">
         <v>13</v>
@@ -1407,12 +1426,17 @@
     </row>
     <row r="35" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>11</v>
+        <v>6</v>
+      </c>
+      <c r="B35" t="s">
+        <v>64</v>
       </c>
       <c r="C35" t="s">
-        <v>66</v>
-      </c>
-      <c r="D35" s="4"/>
+        <v>65</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>13</v>
+      </c>
       <c r="E35" s="4"/>
       <c r="F35" s="1" t="s">
         <v>8</v>
@@ -1424,7 +1448,7 @@
         <v>11</v>
       </c>
       <c r="C36" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D36" s="4"/>
       <c r="E36" s="4"/>
@@ -1438,7 +1462,7 @@
         <v>11</v>
       </c>
       <c r="C37" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D37" s="4"/>
       <c r="E37" s="4"/>
@@ -1452,7 +1476,7 @@
         <v>11</v>
       </c>
       <c r="C38" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D38" s="4"/>
       <c r="E38" s="4"/>
@@ -1466,18 +1490,21 @@
         <v>11</v>
       </c>
       <c r="C39" t="s">
-        <v>70</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="D39" s="4"/>
+      <c r="E39" s="4"/>
       <c r="F39" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="G39" s="4"/>
     </row>
     <row r="40" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C40" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F40" s="1" t="s">
         <v>8</v>
@@ -1488,7 +1515,7 @@
         <v>11</v>
       </c>
       <c r="C41" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F41" s="1" t="s">
         <v>8</v>
@@ -1499,7 +1526,7 @@
         <v>11</v>
       </c>
       <c r="C42" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F42" s="1" t="s">
         <v>8</v>
@@ -1510,13 +1537,19 @@
         <v>11</v>
       </c>
       <c r="C43" t="s">
+        <v>73</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C44" t="s">
         <v>91</v>
       </c>
-      <c r="F43" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="F44" s="1" t="s">
         <v>8</v>
       </c>
@@ -1598,6 +1631,11 @@
     </row>
     <row r="60" spans="6:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="F60" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="61" spans="6:6" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F61" s="1" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added placeholder menus and stuff.
</commit_message>
<xml_diff>
--- a/Doorman_Documents/Asset List.xlsx
+++ b/Doorman_Documents/Asset List.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="107">
   <si>
     <t>Type</t>
   </si>
@@ -337,6 +337,9 @@
   </si>
   <si>
     <t>Hour hand for the clock</t>
+  </si>
+  <si>
+    <t>In-game</t>
   </si>
 </sst>
 </file>
@@ -666,8 +669,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1361,9 +1364,11 @@
       <c r="D31" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E31" s="4"/>
+      <c r="E31" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="F31" s="1" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="G31" s="4"/>
     </row>
@@ -1380,9 +1385,11 @@
       <c r="D32" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E32" s="4"/>
+      <c r="E32" s="4" t="s">
+        <v>106</v>
+      </c>
       <c r="F32" s="1" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="G32" s="4"/>
     </row>
@@ -1399,9 +1406,11 @@
       <c r="D33" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E33" s="4"/>
+      <c r="E33" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="F33" s="1" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="G33" s="4"/>
     </row>
@@ -1418,9 +1427,11 @@
       <c r="D34" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E34" s="4"/>
+      <c r="E34" s="4" t="s">
+        <v>106</v>
+      </c>
       <c r="F34" s="1" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="G34" s="4"/>
     </row>
@@ -1437,9 +1448,11 @@
       <c r="D35" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E35" s="4"/>
+      <c r="E35" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="F35" s="1" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="G35" s="4"/>
     </row>

</xml_diff>

<commit_message>
All game sound/music placeholders added.
</commit_message>
<xml_diff>
--- a/Doorman_Documents/Asset List.xlsx
+++ b/Doorman_Documents/Asset List.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="139">
   <si>
     <t>Type</t>
   </si>
@@ -45,9 +45,6 @@
     <t>Bg_Buttons.jpg</t>
   </si>
   <si>
-    <t>Not Done</t>
-  </si>
-  <si>
     <t>bg</t>
   </si>
   <si>
@@ -376,13 +373,76 @@
   </si>
   <si>
     <t>6.6 sec</t>
+  </si>
+  <si>
+    <t>Text_Lose.jpg</t>
+  </si>
+  <si>
+    <t>Text window for the lose state</t>
+  </si>
+  <si>
+    <t>Text_Win.jpg</t>
+  </si>
+  <si>
+    <t>Text window for the win state</t>
+  </si>
+  <si>
+    <t>882 X 262</t>
+  </si>
+  <si>
+    <t>3.69 sec</t>
+  </si>
+  <si>
+    <t>https://freesound.org/people/LittleRobotSoundFactory/sounds/270329/</t>
+  </si>
+  <si>
+    <t>2.06 sec</t>
+  </si>
+  <si>
+    <t>https://freesound.org/people/kiddpark/sounds/201159/</t>
+  </si>
+  <si>
+    <t>Sound_Lose.wav</t>
+  </si>
+  <si>
+    <t>Sound_Win.mp3</t>
+  </si>
+  <si>
+    <t>music</t>
+  </si>
+  <si>
+    <t>Background music for intro sequence</t>
+  </si>
+  <si>
+    <t>Music_Intro.mp3</t>
+  </si>
+  <si>
+    <t>"Sunflower Dance Party" Kevin MacLeod (incompetech.com) </t>
+  </si>
+  <si>
+    <t>"Deliberate Thought" Kevin MacLeod (incompetech.com) </t>
+  </si>
+  <si>
+    <t>Music_Lobby.mp3</t>
+  </si>
+  <si>
+    <t>"How it Begins" Kevin MacLeod (incompetech.com) </t>
+  </si>
+  <si>
+    <t>Music_Menu.mp3</t>
+  </si>
+  <si>
+    <t>"Satiate - only strings" Kevin MacLeod (incompetech.com) </t>
+  </si>
+  <si>
+    <t>Music_Night.mp3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -391,6 +451,23 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF000000"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -413,7 +490,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -423,6 +500,14 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -703,10 +788,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC61"/>
+  <dimension ref="A1:AC64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -721,13 +806,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
@@ -768,25 +853,25 @@
         <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>18</v>
-      </c>
       <c r="D2" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>9</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -794,22 +879,22 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" t="s">
         <v>19</v>
       </c>
-      <c r="C3" t="s">
-        <v>20</v>
-      </c>
       <c r="D3" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -817,22 +902,22 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s">
         <v>21</v>
       </c>
-      <c r="C4" t="s">
-        <v>22</v>
-      </c>
       <c r="D4" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -843,19 +928,19 @@
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -863,22 +948,22 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" t="s">
         <v>24</v>
       </c>
-      <c r="C6" t="s">
-        <v>25</v>
-      </c>
       <c r="D6" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -886,22 +971,22 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" t="s">
         <v>26</v>
       </c>
-      <c r="C7" t="s">
-        <v>27</v>
-      </c>
       <c r="D7" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -909,19 +994,19 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" t="s">
         <v>28</v>
       </c>
-      <c r="C8" t="s">
-        <v>29</v>
-      </c>
       <c r="D8" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G8" s="4"/>
     </row>
@@ -930,19 +1015,19 @@
         <v>6</v>
       </c>
       <c r="B9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" t="s">
         <v>30</v>
       </c>
-      <c r="C9" t="s">
-        <v>31</v>
-      </c>
       <c r="D9" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G9" s="4"/>
     </row>
@@ -951,19 +1036,19 @@
         <v>6</v>
       </c>
       <c r="B10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" t="s">
         <v>32</v>
       </c>
-      <c r="C10" t="s">
-        <v>33</v>
-      </c>
       <c r="D10" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G10" s="4"/>
     </row>
@@ -972,19 +1057,19 @@
         <v>6</v>
       </c>
       <c r="B11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" t="s">
         <v>34</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D11" s="4" t="s">
-        <v>36</v>
-      </c>
       <c r="E11" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G11" s="4"/>
     </row>
@@ -993,19 +1078,19 @@
         <v>6</v>
       </c>
       <c r="B12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" t="s">
         <v>37</v>
       </c>
-      <c r="C12" t="s">
-        <v>38</v>
-      </c>
       <c r="D12" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G12" s="4"/>
     </row>
@@ -1014,19 +1099,19 @@
         <v>6</v>
       </c>
       <c r="B13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" t="s">
         <v>39</v>
       </c>
-      <c r="C13" t="s">
-        <v>40</v>
-      </c>
       <c r="D13" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G13" s="4"/>
     </row>
@@ -1035,19 +1120,19 @@
         <v>6</v>
       </c>
       <c r="B14" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" t="s">
         <v>41</v>
       </c>
-      <c r="C14" t="s">
-        <v>42</v>
-      </c>
       <c r="D14" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G14" s="4"/>
     </row>
@@ -1056,19 +1141,19 @@
         <v>6</v>
       </c>
       <c r="B15" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" t="s">
         <v>43</v>
       </c>
-      <c r="C15" t="s">
-        <v>44</v>
-      </c>
       <c r="D15" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G15" s="4"/>
     </row>
@@ -1077,19 +1162,19 @@
         <v>6</v>
       </c>
       <c r="B16" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" t="s">
         <v>45</v>
       </c>
-      <c r="C16" t="s">
-        <v>46</v>
-      </c>
       <c r="D16" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G16" s="4"/>
     </row>
@@ -1098,19 +1183,19 @@
         <v>6</v>
       </c>
       <c r="B17" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" t="s">
         <v>47</v>
       </c>
-      <c r="C17" t="s">
-        <v>48</v>
-      </c>
       <c r="D17" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G17" s="4"/>
     </row>
@@ -1119,19 +1204,19 @@
         <v>6</v>
       </c>
       <c r="B18" t="s">
+        <v>73</v>
+      </c>
+      <c r="C18" t="s">
         <v>74</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="D18" s="4" t="s">
-        <v>76</v>
-      </c>
       <c r="E18" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G18" s="4"/>
     </row>
@@ -1140,19 +1225,19 @@
         <v>6</v>
       </c>
       <c r="B19" t="s">
+        <v>91</v>
+      </c>
+      <c r="C19" t="s">
         <v>92</v>
       </c>
-      <c r="C19" t="s">
-        <v>93</v>
-      </c>
       <c r="D19" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G19" s="4"/>
     </row>
@@ -1161,19 +1246,19 @@
         <v>6</v>
       </c>
       <c r="B20" t="s">
+        <v>101</v>
+      </c>
+      <c r="C20" t="s">
         <v>102</v>
       </c>
-      <c r="C20" t="s">
-        <v>103</v>
-      </c>
       <c r="D20" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G20" s="4"/>
     </row>
@@ -1182,19 +1267,19 @@
         <v>6</v>
       </c>
       <c r="B21" t="s">
+        <v>103</v>
+      </c>
+      <c r="C21" t="s">
         <v>104</v>
       </c>
-      <c r="C21" t="s">
-        <v>105</v>
-      </c>
       <c r="D21" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G21" s="4"/>
     </row>
@@ -1203,19 +1288,19 @@
         <v>6</v>
       </c>
       <c r="B22" t="s">
+        <v>76</v>
+      </c>
+      <c r="C22" t="s">
         <v>77</v>
       </c>
-      <c r="C22" t="s">
-        <v>78</v>
-      </c>
       <c r="D22" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G22" s="4"/>
     </row>
@@ -1224,19 +1309,19 @@
         <v>6</v>
       </c>
       <c r="B23" t="s">
+        <v>78</v>
+      </c>
+      <c r="C23" t="s">
         <v>79</v>
       </c>
-      <c r="C23" t="s">
-        <v>80</v>
-      </c>
       <c r="D23" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G23" s="4"/>
     </row>
@@ -1245,19 +1330,19 @@
         <v>6</v>
       </c>
       <c r="B24" t="s">
+        <v>80</v>
+      </c>
+      <c r="C24" t="s">
         <v>81</v>
       </c>
-      <c r="C24" t="s">
-        <v>82</v>
-      </c>
       <c r="D24" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G24" s="4"/>
     </row>
@@ -1266,19 +1351,19 @@
         <v>6</v>
       </c>
       <c r="B25" t="s">
+        <v>82</v>
+      </c>
+      <c r="C25" t="s">
         <v>83</v>
       </c>
-      <c r="C25" t="s">
-        <v>84</v>
-      </c>
       <c r="D25" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G25" s="4"/>
     </row>
@@ -1287,19 +1372,19 @@
         <v>6</v>
       </c>
       <c r="B26" t="s">
+        <v>84</v>
+      </c>
+      <c r="C26" t="s">
         <v>85</v>
       </c>
-      <c r="C26" t="s">
-        <v>86</v>
-      </c>
       <c r="D26" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G26" s="4"/>
     </row>
@@ -1308,19 +1393,19 @@
         <v>6</v>
       </c>
       <c r="B27" t="s">
+        <v>86</v>
+      </c>
+      <c r="C27" t="s">
         <v>87</v>
       </c>
-      <c r="C27" t="s">
-        <v>88</v>
-      </c>
       <c r="D27" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G27" s="4"/>
     </row>
@@ -1329,61 +1414,61 @@
         <v>6</v>
       </c>
       <c r="B28" t="s">
+        <v>88</v>
+      </c>
+      <c r="C28" t="s">
         <v>89</v>
       </c>
-      <c r="C28" t="s">
-        <v>90</v>
-      </c>
       <c r="D28" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G28" s="4"/>
     </row>
-    <row r="29" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B29" t="s">
-        <v>49</v>
+        <v>118</v>
       </c>
       <c r="C29" t="s">
-        <v>50</v>
+        <v>119</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>51</v>
+        <v>122</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>52</v>
+        <v>13</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="G29" s="4"/>
     </row>
-    <row r="30" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B30" t="s">
-        <v>53</v>
+        <v>120</v>
       </c>
       <c r="C30" t="s">
-        <v>54</v>
+        <v>121</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>55</v>
+        <v>122</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>52</v>
+        <v>13</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="G30" s="4"/>
     </row>
@@ -1392,19 +1477,19 @@
         <v>6</v>
       </c>
       <c r="B31" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="C31" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>13</v>
+        <v>50</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>15</v>
+        <v>51</v>
       </c>
       <c r="G31" s="4"/>
     </row>
@@ -1413,19 +1498,19 @@
         <v>6</v>
       </c>
       <c r="B32" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C32" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>13</v>
+        <v>54</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>106</v>
+        <v>13</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>15</v>
+        <v>51</v>
       </c>
       <c r="G32" s="4"/>
     </row>
@@ -1434,19 +1519,19 @@
         <v>6</v>
       </c>
       <c r="B33" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C33" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G33" s="4"/>
     </row>
@@ -1455,19 +1540,19 @@
         <v>6</v>
       </c>
       <c r="B34" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C34" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G34" s="4"/>
     </row>
@@ -1476,253 +1561,322 @@
         <v>6</v>
       </c>
       <c r="B35" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C35" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G35" s="4"/>
     </row>
     <row r="36" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>11</v>
+        <v>6</v>
+      </c>
+      <c r="B36" t="s">
+        <v>61</v>
       </c>
       <c r="C36" t="s">
-        <v>66</v>
-      </c>
-      <c r="D36" s="4"/>
-      <c r="E36" s="4"/>
+        <v>62</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>105</v>
+      </c>
       <c r="F36" s="1" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="G36" s="4"/>
     </row>
     <row r="37" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>11</v>
+        <v>6</v>
+      </c>
+      <c r="B37" t="s">
+        <v>63</v>
       </c>
       <c r="C37" t="s">
-        <v>67</v>
-      </c>
-      <c r="D37" s="4"/>
-      <c r="E37" s="4"/>
+        <v>64</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>13</v>
+      </c>
       <c r="F37" s="1" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="G37" s="4"/>
     </row>
     <row r="38" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>11</v>
+        <v>129</v>
+      </c>
+      <c r="B38" s="8" t="s">
+        <v>136</v>
       </c>
       <c r="C38" t="s">
-        <v>68</v>
-      </c>
-      <c r="D38" s="4"/>
-      <c r="E38" s="4"/>
-      <c r="F38" s="1" t="s">
-        <v>8</v>
+        <v>65</v>
+      </c>
+      <c r="D38" s="7">
+        <v>0.13194444444444445</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="F38" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="G38" s="4"/>
     </row>
     <row r="39" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>11</v>
+        <v>129</v>
       </c>
       <c r="B39" t="s">
-        <v>107</v>
+        <v>131</v>
       </c>
       <c r="C39" t="s">
-        <v>69</v>
-      </c>
-      <c r="D39" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="E39" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>15</v>
+        <v>130</v>
+      </c>
+      <c r="D39" s="7">
+        <v>0.2388888888888889</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="F39" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="G39" s="4"/>
     </row>
     <row r="40" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>11</v>
+        <v>129</v>
+      </c>
+      <c r="B40" s="8" t="s">
+        <v>134</v>
       </c>
       <c r="C40" t="s">
-        <v>70</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>8</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="D40" s="7">
+        <v>0.12291666666666667</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="F40" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G40" s="4"/>
     </row>
     <row r="41" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>11</v>
+        <v>129</v>
+      </c>
+      <c r="B41" s="8" t="s">
+        <v>138</v>
       </c>
       <c r="C41" t="s">
-        <v>71</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>8</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="D41" s="7">
+        <v>0.13333333333333333</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="F41" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G41" s="4"/>
     </row>
     <row r="42" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B42" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="C42" t="s">
-        <v>72</v>
-      </c>
-      <c r="D42" t="s">
-        <v>115</v>
-      </c>
-      <c r="E42" t="s">
-        <v>114</v>
+        <v>68</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>108</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>15</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="G42" s="4"/>
     </row>
     <row r="43" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B43" t="s">
-        <v>111</v>
+        <v>127</v>
       </c>
       <c r="C43" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D43" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
       <c r="E43" t="s">
-        <v>110</v>
+        <v>124</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B44" t="s">
-        <v>108</v>
+        <v>128</v>
       </c>
       <c r="C44" t="s">
-        <v>91</v>
+        <v>70</v>
       </c>
       <c r="D44" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="E44" t="s">
+        <v>126</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A45" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B45" t="s">
         <v>112</v>
       </c>
-      <c r="F44" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="C45" t="s">
+        <v>71</v>
+      </c>
+      <c r="D45" t="s">
+        <v>114</v>
+      </c>
+      <c r="E45" t="s">
+        <v>113</v>
+      </c>
       <c r="F45" s="1" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A46" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B46" t="s">
+        <v>110</v>
+      </c>
+      <c r="C46" t="s">
+        <v>72</v>
+      </c>
+      <c r="D46" t="s">
+        <v>115</v>
+      </c>
+      <c r="E46" t="s">
+        <v>109</v>
+      </c>
       <c r="F46" s="1" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A47" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B47" t="s">
+        <v>107</v>
+      </c>
+      <c r="C47" t="s">
+        <v>90</v>
+      </c>
+      <c r="D47" t="s">
+        <v>116</v>
+      </c>
+      <c r="E47" t="s">
+        <v>111</v>
+      </c>
       <c r="F47" s="1" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="F48" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="F48" s="1"/>
     </row>
     <row r="49" spans="6:6" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="F49" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="F49" s="1"/>
     </row>
     <row r="50" spans="6:6" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="F50" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="F50" s="1"/>
     </row>
     <row r="51" spans="6:6" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="F51" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="F51" s="1"/>
     </row>
     <row r="52" spans="6:6" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="F52" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="F52" s="1"/>
     </row>
     <row r="53" spans="6:6" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="F53" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="F53" s="1"/>
     </row>
     <row r="54" spans="6:6" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="F54" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="F54" s="1"/>
     </row>
     <row r="55" spans="6:6" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="F55" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="F55" s="1"/>
     </row>
     <row r="56" spans="6:6" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="F56" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="F56" s="1"/>
     </row>
     <row r="57" spans="6:6" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="F57" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="F57" s="1"/>
     </row>
     <row r="58" spans="6:6" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="F58" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="F58" s="1"/>
     </row>
     <row r="59" spans="6:6" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="F59" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="F59" s="1"/>
     </row>
     <row r="60" spans="6:6" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="F60" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="F60" s="1"/>
     </row>
     <row r="61" spans="6:6" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="F61" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="F61" s="1"/>
+    </row>
+    <row r="62" spans="6:6" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F62" s="1"/>
+    </row>
+    <row r="63" spans="6:6" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F63" s="1"/>
+    </row>
+    <row r="64" spans="6:6" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F64" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added bg_City, defined remaining images in script and put under labels.
</commit_message>
<xml_diff>
--- a/Doorman_Documents/Asset List.xlsx
+++ b/Doorman_Documents/Asset List.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="142">
   <si>
     <t>Type</t>
   </si>
@@ -436,6 +436,15 @@
   </si>
   <si>
     <t>Music_Night.mp3</t>
+  </si>
+  <si>
+    <t>Bg_City.jpg</t>
+  </si>
+  <si>
+    <t>3840 X 1080</t>
+  </si>
+  <si>
+    <t>City BG for panning.</t>
   </si>
 </sst>
 </file>
@@ -788,10 +797,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC64"/>
+  <dimension ref="A1:AC65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1057,18 +1066,18 @@
         <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>33</v>
+        <v>139</v>
       </c>
       <c r="C11" t="s">
-        <v>34</v>
+        <v>141</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>35</v>
+        <v>140</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="F11" s="2" t="s">
         <v>14</v>
       </c>
       <c r="G11" s="4"/>
@@ -1078,10 +1087,10 @@
         <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C12" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>35</v>
@@ -1099,10 +1108,10 @@
         <v>6</v>
       </c>
       <c r="B13" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C13" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>35</v>
@@ -1120,10 +1129,10 @@
         <v>6</v>
       </c>
       <c r="B14" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C14" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>35</v>
@@ -1141,10 +1150,10 @@
         <v>6</v>
       </c>
       <c r="B15" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C15" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>35</v>
@@ -1162,10 +1171,10 @@
         <v>6</v>
       </c>
       <c r="B16" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C16" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>35</v>
@@ -1183,10 +1192,10 @@
         <v>6</v>
       </c>
       <c r="B17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C17" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>35</v>
@@ -1204,18 +1213,18 @@
         <v>6</v>
       </c>
       <c r="B18" t="s">
-        <v>73</v>
+        <v>46</v>
       </c>
       <c r="C18" t="s">
-        <v>74</v>
+        <v>47</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>75</v>
+        <v>35</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F18" s="2" t="s">
+      <c r="F18" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G18" s="4"/>
@@ -1225,13 +1234,13 @@
         <v>6</v>
       </c>
       <c r="B19" t="s">
-        <v>91</v>
+        <v>73</v>
       </c>
       <c r="C19" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="E19" s="4" t="s">
         <v>13</v>
@@ -1246,10 +1255,10 @@
         <v>6</v>
       </c>
       <c r="B20" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="C20" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>100</v>
@@ -1267,10 +1276,10 @@
         <v>6</v>
       </c>
       <c r="B21" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C21" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>100</v>
@@ -1288,13 +1297,13 @@
         <v>6</v>
       </c>
       <c r="B22" t="s">
-        <v>76</v>
+        <v>103</v>
       </c>
       <c r="C22" t="s">
-        <v>77</v>
+        <v>104</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="E22" s="4" t="s">
         <v>13</v>
@@ -1309,13 +1318,13 @@
         <v>6</v>
       </c>
       <c r="B23" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C23" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E23" s="4" t="s">
         <v>13</v>
@@ -1330,13 +1339,13 @@
         <v>6</v>
       </c>
       <c r="B24" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C24" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E24" s="4" t="s">
         <v>13</v>
@@ -1351,13 +1360,13 @@
         <v>6</v>
       </c>
       <c r="B25" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C25" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E25" s="4" t="s">
         <v>13</v>
@@ -1372,13 +1381,13 @@
         <v>6</v>
       </c>
       <c r="B26" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C26" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E26" s="4" t="s">
         <v>13</v>
@@ -1393,13 +1402,13 @@
         <v>6</v>
       </c>
       <c r="B27" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C27" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E27" s="4" t="s">
         <v>13</v>
@@ -1414,13 +1423,13 @@
         <v>6</v>
       </c>
       <c r="B28" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C28" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E28" s="4" t="s">
         <v>13</v>
@@ -1435,13 +1444,13 @@
         <v>6</v>
       </c>
       <c r="B29" t="s">
-        <v>118</v>
+        <v>88</v>
       </c>
       <c r="C29" t="s">
-        <v>119</v>
+        <v>89</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>122</v>
+        <v>99</v>
       </c>
       <c r="E29" s="4" t="s">
         <v>13</v>
@@ -1456,10 +1465,10 @@
         <v>6</v>
       </c>
       <c r="B30" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C30" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D30" s="4" t="s">
         <v>122</v>
@@ -1472,24 +1481,24 @@
       </c>
       <c r="G30" s="4"/>
     </row>
-    <row r="31" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B31" t="s">
-        <v>48</v>
+        <v>120</v>
       </c>
       <c r="C31" t="s">
-        <v>49</v>
+        <v>121</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>50</v>
+        <v>122</v>
       </c>
       <c r="E31" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F31" s="1" t="s">
-        <v>51</v>
+      <c r="F31" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="G31" s="4"/>
     </row>
@@ -1498,13 +1507,13 @@
         <v>6</v>
       </c>
       <c r="B32" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C32" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E32" s="4" t="s">
         <v>13</v>
@@ -1519,19 +1528,19 @@
         <v>6</v>
       </c>
       <c r="B33" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C33" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="E33" s="4" t="s">
         <v>13</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>14</v>
+        <v>51</v>
       </c>
       <c r="G33" s="4"/>
     </row>
@@ -1540,16 +1549,16 @@
         <v>6</v>
       </c>
       <c r="B34" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C34" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D34" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>105</v>
+        <v>13</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>14</v>
@@ -1561,16 +1570,16 @@
         <v>6</v>
       </c>
       <c r="B35" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C35" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D35" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>13</v>
+        <v>105</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>14</v>
@@ -1582,16 +1591,16 @@
         <v>6</v>
       </c>
       <c r="B36" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C36" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D36" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>105</v>
+        <v>13</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>14</v>
@@ -1603,16 +1612,16 @@
         <v>6</v>
       </c>
       <c r="B37" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C37" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D37" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>13</v>
+        <v>105</v>
       </c>
       <c r="F37" s="1" t="s">
         <v>14</v>
@@ -1621,21 +1630,21 @@
     </row>
     <row r="38" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="B38" s="8" t="s">
-        <v>136</v>
+        <v>6</v>
+      </c>
+      <c r="B38" t="s">
+        <v>63</v>
       </c>
       <c r="C38" t="s">
-        <v>65</v>
-      </c>
-      <c r="D38" s="7">
-        <v>0.13194444444444445</v>
-      </c>
-      <c r="E38" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="F38" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F38" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G38" s="4"/>
@@ -1644,17 +1653,17 @@
       <c r="A39" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="B39" t="s">
-        <v>131</v>
+      <c r="B39" s="8" t="s">
+        <v>136</v>
       </c>
       <c r="C39" t="s">
-        <v>130</v>
+        <v>65</v>
       </c>
       <c r="D39" s="7">
-        <v>0.2388888888888889</v>
+        <v>0.13194444444444445</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="F39" s="6" t="s">
         <v>14</v>
@@ -1665,17 +1674,17 @@
       <c r="A40" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="B40" s="8" t="s">
-        <v>134</v>
+      <c r="B40" t="s">
+        <v>131</v>
       </c>
       <c r="C40" t="s">
-        <v>66</v>
+        <v>130</v>
       </c>
       <c r="D40" s="7">
-        <v>0.12291666666666667</v>
+        <v>0.2388888888888889</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F40" s="6" t="s">
         <v>14</v>
@@ -1687,16 +1696,16 @@
         <v>129</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C41" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D41" s="7">
-        <v>0.13333333333333333</v>
+        <v>0.12291666666666667</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="F41" s="6" t="s">
         <v>14</v>
@@ -1705,21 +1714,21 @@
     </row>
     <row r="42" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B42" t="s">
-        <v>106</v>
+        <v>129</v>
+      </c>
+      <c r="B42" s="8" t="s">
+        <v>138</v>
       </c>
       <c r="C42" t="s">
-        <v>68</v>
-      </c>
-      <c r="D42" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="E42" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="F42" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D42" s="7">
+        <v>0.13333333333333333</v>
+      </c>
+      <c r="E42" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="F42" s="6" t="s">
         <v>14</v>
       </c>
       <c r="G42" s="4"/>
@@ -1729,36 +1738,37 @@
         <v>10</v>
       </c>
       <c r="B43" t="s">
-        <v>127</v>
+        <v>106</v>
       </c>
       <c r="C43" t="s">
-        <v>69</v>
-      </c>
-      <c r="D43" t="s">
-        <v>123</v>
-      </c>
-      <c r="E43" t="s">
-        <v>124</v>
+        <v>68</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="E43" s="4" t="s">
+        <v>108</v>
       </c>
       <c r="F43" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="G43" s="4"/>
     </row>
     <row r="44" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B44" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C44" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D44" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E44" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F44" s="1" t="s">
         <v>14</v>
@@ -1769,16 +1779,16 @@
         <v>10</v>
       </c>
       <c r="B45" t="s">
-        <v>112</v>
+        <v>128</v>
       </c>
       <c r="C45" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D45" t="s">
-        <v>114</v>
+        <v>125</v>
       </c>
       <c r="E45" t="s">
-        <v>113</v>
+        <v>126</v>
       </c>
       <c r="F45" s="1" t="s">
         <v>14</v>
@@ -1789,16 +1799,16 @@
         <v>10</v>
       </c>
       <c r="B46" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="C46" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D46" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E46" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="F46" s="1" t="s">
         <v>14</v>
@@ -1809,23 +1819,40 @@
         <v>10</v>
       </c>
       <c r="B47" t="s">
+        <v>110</v>
+      </c>
+      <c r="C47" t="s">
+        <v>72</v>
+      </c>
+      <c r="D47" t="s">
+        <v>115</v>
+      </c>
+      <c r="E47" t="s">
+        <v>109</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A48" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B48" t="s">
         <v>107</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C48" t="s">
         <v>90</v>
       </c>
-      <c r="D47" t="s">
+      <c r="D48" t="s">
         <v>116</v>
       </c>
-      <c r="E47" t="s">
+      <c r="E48" t="s">
         <v>111</v>
       </c>
-      <c r="F47" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="F48" s="1"/>
+      <c r="F48" s="1" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="49" spans="6:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="F49" s="1"/>
@@ -1874,6 +1901,9 @@
     </row>
     <row r="64" spans="6:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="F64" s="1"/>
+    </row>
+    <row r="65" spans="6:6" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F65" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Character art finished, asset list updated.
</commit_message>
<xml_diff>
--- a/Doorman_Documents/Asset List.xlsx
+++ b/Doorman_Documents/Asset List.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kyle\Documents\The_Doorman\Doorman_Documents\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23680" windowHeight="16040"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23676" windowHeight="16044"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="216">
   <si>
     <t>flour</t>
     <phoneticPr fontId="5" type="noConversion"/>
@@ -240,10 +245,6 @@
   </si>
   <si>
     <t>image by Baiey</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>Final</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
@@ -749,14 +750,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -1097,53 +1092,53 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr published="0"/>
   <dimension ref="A1:AC67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D27" workbookViewId="0">
-      <selection activeCell="G40" sqref="G40"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.1640625" customWidth="1"/>
+    <col min="1" max="1" width="12.109375" customWidth="1"/>
     <col min="2" max="2" width="32.33203125" customWidth="1"/>
     <col min="3" max="3" width="43.6640625" customWidth="1"/>
     <col min="5" max="5" width="57" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="15.75" customHeight="1">
+    <row r="1" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>144</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>145</v>
       </c>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
@@ -1167,180 +1162,180 @@
       <c r="AB1" s="2"/>
       <c r="AC1" s="2"/>
     </row>
-    <row r="2" spans="1:29" ht="15.75" customHeight="1">
+    <row r="2" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>156</v>
-      </c>
       <c r="D2" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>153</v>
+        <v>189</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:29" ht="15.75" customHeight="1">
+    <row r="3" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B3" t="s">
+        <v>156</v>
+      </c>
+      <c r="C3" t="s">
         <v>157</v>
       </c>
-      <c r="C3" t="s">
-        <v>158</v>
-      </c>
       <c r="D3" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>153</v>
+        <v>189</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H3" s="9" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:29" ht="15.75" customHeight="1">
+    <row r="4" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B4" t="s">
+        <v>158</v>
+      </c>
+      <c r="C4" t="s">
         <v>159</v>
       </c>
-      <c r="C4" t="s">
-        <v>160</v>
-      </c>
       <c r="D4" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H4" s="4" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:29" ht="15.75" customHeight="1">
+    <row r="5" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="B5" t="s">
         <v>146</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
+        <v>160</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="G5" s="4" t="s">
         <v>147</v>
-      </c>
-      <c r="C5" t="s">
-        <v>161</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>148</v>
       </c>
       <c r="H5" s="4" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:29" ht="15.75" customHeight="1">
+    <row r="6" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B6" t="s">
+        <v>161</v>
+      </c>
+      <c r="C6" t="s">
         <v>162</v>
       </c>
-      <c r="C6" t="s">
-        <v>163</v>
-      </c>
       <c r="D6" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H6" s="4" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:29" ht="15.75" customHeight="1">
+    <row r="7" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B7" t="s">
+        <v>163</v>
+      </c>
+      <c r="C7" t="s">
         <v>164</v>
       </c>
-      <c r="C7" t="s">
-        <v>165</v>
-      </c>
       <c r="D7" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H7" s="4" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:29" ht="15.75" customHeight="1">
+    <row r="8" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B8" t="s">
+        <v>165</v>
+      </c>
+      <c r="C8" t="s">
         <v>166</v>
       </c>
-      <c r="C8" t="s">
-        <v>167</v>
-      </c>
       <c r="D8" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>38</v>
@@ -1349,15 +1344,15 @@
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:29" ht="15.75" customHeight="1">
+    <row r="9" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="B9" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="C9" s="9" t="s">
         <v>138</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>139</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>35</v>
@@ -1375,12 +1370,12 @@
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:29" ht="15.75" customHeight="1">
+    <row r="10" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>54</v>
@@ -1392,76 +1387,76 @@
         <v>55</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>56</v>
+        <v>189</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>38</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="11" spans="1:29" ht="15.75" customHeight="1">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B11" t="s">
+        <v>167</v>
+      </c>
+      <c r="C11" t="s">
         <v>168</v>
       </c>
-      <c r="C11" t="s">
-        <v>169</v>
-      </c>
       <c r="D11" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>38</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="12" spans="1:29" ht="15.75" customHeight="1">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B12" t="s">
+        <v>169</v>
+      </c>
+      <c r="C12" t="s">
         <v>170</v>
       </c>
-      <c r="C12" t="s">
-        <v>171</v>
-      </c>
       <c r="D12" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G12" s="4" t="s">
         <v>38</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="13" spans="1:29" ht="15.75" customHeight="1">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B13" t="s">
+        <v>60</v>
+      </c>
+      <c r="C13" s="9" t="s">
         <v>61</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>62</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>35</v>
@@ -1476,339 +1471,339 @@
         <v>38</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="14" spans="1:29" ht="15.75" customHeight="1">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B14" t="s">
+        <v>171</v>
+      </c>
+      <c r="C14" t="s">
         <v>172</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="D14" s="4" t="s">
-        <v>174</v>
-      </c>
       <c r="E14" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>153</v>
+        <v>189</v>
       </c>
       <c r="G14" s="4" t="s">
         <v>39</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="15" spans="1:29" ht="15.75" customHeight="1">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B15" t="s">
+        <v>174</v>
+      </c>
+      <c r="C15" t="s">
         <v>175</v>
       </c>
-      <c r="C15" t="s">
-        <v>176</v>
-      </c>
       <c r="D15" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>153</v>
+        <v>189</v>
       </c>
       <c r="G15" s="4" t="s">
         <v>39</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="16" spans="1:29" ht="15.75" customHeight="1">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B16" t="s">
+        <v>176</v>
+      </c>
+      <c r="C16" t="s">
         <v>177</v>
       </c>
-      <c r="C16" t="s">
-        <v>178</v>
-      </c>
       <c r="D16" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>153</v>
+        <v>189</v>
       </c>
       <c r="G16" s="4" t="s">
         <v>39</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="15.75" customHeight="1">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B17" t="s">
+        <v>178</v>
+      </c>
+      <c r="C17" t="s">
         <v>179</v>
       </c>
-      <c r="C17" t="s">
-        <v>180</v>
-      </c>
       <c r="D17" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>153</v>
+        <v>189</v>
       </c>
       <c r="G17" s="4" t="s">
         <v>39</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="15.75" customHeight="1">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B18" t="s">
+        <v>180</v>
+      </c>
+      <c r="C18" t="s">
         <v>181</v>
       </c>
-      <c r="C18" t="s">
-        <v>182</v>
-      </c>
       <c r="D18" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>153</v>
+        <v>189</v>
       </c>
       <c r="G18" s="4" t="s">
         <v>40</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="15.75" customHeight="1">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B19" t="s">
+        <v>182</v>
+      </c>
+      <c r="C19" t="s">
         <v>183</v>
       </c>
-      <c r="C19" t="s">
-        <v>184</v>
-      </c>
       <c r="D19" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>153</v>
+        <v>189</v>
       </c>
       <c r="G19" s="4" t="s">
         <v>40</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="15.75" customHeight="1">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B20" t="s">
+        <v>184</v>
+      </c>
+      <c r="C20" t="s">
         <v>185</v>
       </c>
-      <c r="C20" t="s">
-        <v>186</v>
-      </c>
       <c r="D20" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>153</v>
+        <v>189</v>
       </c>
       <c r="G20" s="4" t="s">
         <v>39</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="15.75" customHeight="1">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B21" t="s">
+        <v>211</v>
+      </c>
+      <c r="C21" t="s">
         <v>212</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" s="4" t="s">
         <v>213</v>
       </c>
-      <c r="D21" s="4" t="s">
-        <v>214</v>
-      </c>
       <c r="E21" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G21" s="4" t="s">
         <v>41</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="15.75" customHeight="1">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B22" t="s">
+        <v>88</v>
+      </c>
+      <c r="C22" t="s">
         <v>89</v>
       </c>
-      <c r="C22" t="s">
-        <v>90</v>
-      </c>
       <c r="D22" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G22" s="4" t="s">
         <v>41</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="15.75" customHeight="1">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B23" t="s">
+        <v>98</v>
+      </c>
+      <c r="C23" t="s">
         <v>99</v>
       </c>
-      <c r="C23" t="s">
-        <v>100</v>
-      </c>
       <c r="D23" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G23" s="4" t="s">
         <v>41</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="15.75" customHeight="1">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B24" t="s">
+        <v>100</v>
+      </c>
+      <c r="C24" t="s">
         <v>101</v>
       </c>
-      <c r="C24" t="s">
-        <v>102</v>
-      </c>
       <c r="D24" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G24" s="4" t="s">
         <v>41</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="15.75" customHeight="1">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B25" t="s">
+        <v>214</v>
+      </c>
+      <c r="C25" t="s">
         <v>215</v>
       </c>
-      <c r="C25" t="s">
-        <v>216</v>
-      </c>
       <c r="D25" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G25" s="4" t="s">
         <v>41</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="15.75" customHeight="1">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B26" t="s">
+        <v>75</v>
+      </c>
+      <c r="C26" t="s">
         <v>76</v>
       </c>
-      <c r="C26" t="s">
-        <v>77</v>
-      </c>
       <c r="D26" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G26" s="4" t="s">
         <v>41</v>
@@ -1817,24 +1812,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="15.75" customHeight="1">
+    <row r="27" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B27" t="s">
+        <v>77</v>
+      </c>
+      <c r="C27" t="s">
         <v>78</v>
       </c>
-      <c r="C27" t="s">
-        <v>79</v>
-      </c>
       <c r="D27" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G27" s="4" t="s">
         <v>42</v>
@@ -1843,24 +1838,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="15.75" customHeight="1">
+    <row r="28" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B28" t="s">
+        <v>79</v>
+      </c>
+      <c r="C28" t="s">
         <v>80</v>
       </c>
-      <c r="C28" t="s">
-        <v>81</v>
-      </c>
       <c r="D28" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G28" s="4" t="s">
         <v>43</v>
@@ -1869,24 +1864,24 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="15.75" customHeight="1">
+    <row r="29" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B29" t="s">
+        <v>81</v>
+      </c>
+      <c r="C29" t="s">
         <v>82</v>
       </c>
-      <c r="C29" t="s">
-        <v>83</v>
-      </c>
       <c r="D29" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G29" s="4" t="s">
         <v>41</v>
@@ -1895,24 +1890,24 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="15.75" customHeight="1">
+    <row r="30" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B30" t="s">
+        <v>83</v>
+      </c>
+      <c r="C30" t="s">
         <v>84</v>
       </c>
-      <c r="C30" t="s">
-        <v>85</v>
-      </c>
       <c r="D30" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G30" s="4" t="s">
         <v>41</v>
@@ -1921,24 +1916,24 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="15.75" customHeight="1">
+    <row r="31" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B31" t="s">
+        <v>85</v>
+      </c>
+      <c r="C31" t="s">
         <v>86</v>
       </c>
-      <c r="C31" t="s">
-        <v>87</v>
-      </c>
       <c r="D31" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G31" s="4" t="s">
         <v>41</v>
@@ -1947,24 +1942,24 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="15.75" customHeight="1">
+    <row r="32" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B32" t="s">
+        <v>115</v>
+      </c>
+      <c r="C32" t="s">
         <v>116</v>
       </c>
-      <c r="C32" t="s">
-        <v>117</v>
-      </c>
       <c r="D32" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G32" s="4" t="s">
         <v>34</v>
@@ -1973,24 +1968,24 @@
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="15.75" customHeight="1">
+    <row r="33" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B33" t="s">
+        <v>117</v>
+      </c>
+      <c r="C33" t="s">
         <v>118</v>
       </c>
-      <c r="C33" t="s">
+      <c r="D33" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="D33" s="4" t="s">
-        <v>120</v>
-      </c>
       <c r="E33" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G33" s="4" t="s">
         <v>34</v>
@@ -1999,24 +1994,24 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="12">
+    <row r="34" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B34" t="s">
+        <v>186</v>
+      </c>
+      <c r="C34" t="s">
         <v>187</v>
       </c>
-      <c r="C34" t="s">
+      <c r="D34" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="D34" s="4" t="s">
+      <c r="E34" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="F34" s="1" t="s">
         <v>189</v>
-      </c>
-      <c r="E34" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>190</v>
       </c>
       <c r="G34" s="4" t="s">
         <v>44</v>
@@ -2025,24 +2020,24 @@
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="12">
+    <row r="35" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B35" t="s">
+        <v>190</v>
+      </c>
+      <c r="C35" t="s">
         <v>191</v>
       </c>
-      <c r="C35" t="s">
+      <c r="D35" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="D35" s="4" t="s">
-        <v>193</v>
-      </c>
       <c r="E35" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G35" s="4" t="s">
         <v>45</v>
@@ -2051,24 +2046,24 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="12">
+    <row r="36" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B36" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C36" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G36" s="4" t="s">
         <v>34</v>
@@ -2077,24 +2072,24 @@
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="12">
+    <row r="37" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B37" t="s">
+        <v>195</v>
+      </c>
+      <c r="C37" t="s">
         <v>196</v>
       </c>
-      <c r="C37" t="s">
-        <v>197</v>
-      </c>
       <c r="D37" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G37" s="4" t="s">
         <v>34</v>
@@ -2103,24 +2098,24 @@
         <v>11</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="12">
+    <row r="38" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B38" t="s">
+        <v>197</v>
+      </c>
+      <c r="C38" t="s">
         <v>198</v>
       </c>
-      <c r="C38" t="s">
-        <v>199</v>
-      </c>
       <c r="D38" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G38" s="4" t="s">
         <v>34</v>
@@ -2129,24 +2124,24 @@
         <v>12</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="12">
+    <row r="39" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B39" t="s">
+        <v>199</v>
+      </c>
+      <c r="C39" t="s">
         <v>200</v>
       </c>
-      <c r="C39" t="s">
-        <v>201</v>
-      </c>
       <c r="D39" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G39" s="4" t="s">
         <v>34</v>
@@ -2155,24 +2150,24 @@
         <v>13</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="12">
+    <row r="40" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B40" t="s">
+        <v>201</v>
+      </c>
+      <c r="C40" t="s">
         <v>202</v>
       </c>
-      <c r="C40" t="s">
-        <v>203</v>
-      </c>
       <c r="D40" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G40" s="4" t="s">
         <v>34</v>
@@ -2181,24 +2176,24 @@
         <v>14</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="12">
+    <row r="41" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C41" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D41" s="7">
         <v>0.13194444444444445</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F41" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G41" s="2" t="s">
         <v>15</v>
@@ -2207,24 +2202,24 @@
         <v>26</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="12">
+    <row r="42" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="B42" t="s">
+        <v>128</v>
+      </c>
+      <c r="C42" t="s">
         <v>127</v>
-      </c>
-      <c r="B42" t="s">
-        <v>129</v>
-      </c>
-      <c r="C42" t="s">
-        <v>128</v>
       </c>
       <c r="D42" s="7">
         <v>0.2388888888888889</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F42" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G42" s="2" t="s">
         <v>15</v>
@@ -2233,24 +2228,24 @@
         <v>27</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="12">
+    <row r="43" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C43" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D43" s="7">
         <v>0.12291666666666667</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F43" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G43" s="2" t="s">
         <v>15</v>
@@ -2259,24 +2254,24 @@
         <v>28</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="12">
+    <row r="44" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C44" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D44" s="7">
         <v>0.13333333333333333</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F44" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G44" s="2" t="s">
         <v>15</v>
@@ -2285,24 +2280,24 @@
         <v>29</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="12">
+    <row r="45" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B45" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C45" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G45" s="2" t="s">
         <v>15</v>
@@ -2311,24 +2306,24 @@
         <v>30</v>
       </c>
     </row>
-    <row r="46" spans="1:8" ht="12">
+    <row r="46" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B46" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C46" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D46" t="s">
+        <v>120</v>
+      </c>
+      <c r="E46" t="s">
         <v>121</v>
       </c>
-      <c r="E46" t="s">
-        <v>122</v>
-      </c>
       <c r="F46" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G46" s="2" t="s">
         <v>16</v>
@@ -2337,24 +2332,24 @@
         <v>31</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="12">
+    <row r="47" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B47" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C47" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D47" t="s">
+        <v>122</v>
+      </c>
+      <c r="E47" t="s">
         <v>123</v>
       </c>
-      <c r="E47" t="s">
-        <v>124</v>
-      </c>
       <c r="F47" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G47" s="2" t="s">
         <v>16</v>
@@ -2363,24 +2358,24 @@
         <v>32</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="12">
+    <row r="48" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B48" t="s">
+        <v>109</v>
+      </c>
+      <c r="C48" t="s">
+        <v>209</v>
+      </c>
+      <c r="D48" t="s">
+        <v>111</v>
+      </c>
+      <c r="E48" t="s">
         <v>110</v>
       </c>
-      <c r="C48" t="s">
-        <v>210</v>
-      </c>
-      <c r="D48" t="s">
-        <v>112</v>
-      </c>
-      <c r="E48" t="s">
-        <v>111</v>
-      </c>
       <c r="F48" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G48" s="2" t="s">
         <v>16</v>
@@ -2389,24 +2384,24 @@
         <v>33</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="12">
+    <row r="49" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B49" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C49" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D49" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E49" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G49" s="2" t="s">
         <v>15</v>
@@ -2415,24 +2410,24 @@
         <v>25</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="12">
+    <row r="50" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B50" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C50" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D50" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E50" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G50" s="2" t="s">
         <v>16</v>
@@ -2441,7 +2436,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="51" spans="1:8" ht="12">
+    <row r="51" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>17</v>
       </c>
@@ -2467,52 +2462,52 @@
         <v>23</v>
       </c>
     </row>
-    <row r="52" spans="1:8" ht="12">
+    <row r="52" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="F52" s="1"/>
     </row>
-    <row r="53" spans="1:8" ht="12">
+    <row r="53" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="F53" s="1"/>
     </row>
-    <row r="54" spans="1:8" ht="12">
+    <row r="54" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="F54" s="1"/>
     </row>
-    <row r="55" spans="1:8" ht="12">
+    <row r="55" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="F55" s="1"/>
     </row>
-    <row r="56" spans="1:8" ht="12">
+    <row r="56" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="F56" s="1"/>
     </row>
-    <row r="57" spans="1:8" ht="12">
+    <row r="57" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="F57" s="1"/>
     </row>
-    <row r="58" spans="1:8" ht="12">
+    <row r="58" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="F58" s="1"/>
     </row>
-    <row r="59" spans="1:8" ht="12">
+    <row r="59" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="F59" s="1"/>
     </row>
-    <row r="60" spans="1:8" ht="12">
+    <row r="60" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="F60" s="1"/>
     </row>
-    <row r="61" spans="1:8" ht="12">
+    <row r="61" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="F61" s="1"/>
     </row>
-    <row r="62" spans="1:8" ht="12">
+    <row r="62" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="F62" s="1"/>
     </row>
-    <row r="63" spans="1:8" ht="12">
+    <row r="63" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="F63" s="1"/>
     </row>
-    <row r="64" spans="1:8" ht="12">
+    <row r="64" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="F64" s="1"/>
     </row>
-    <row r="65" spans="6:6" ht="12">
+    <row r="65" spans="6:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="F65" s="1"/>
     </row>
-    <row r="66" spans="6:6" ht="12">
+    <row r="66" spans="6:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="F66" s="1"/>
     </row>
-    <row r="67" spans="6:6" ht="12">
+    <row r="67" spans="6:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="F67" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Hotel BG's done minus the hallway/door images. Updated Asset List.
</commit_message>
<xml_diff>
--- a/Doorman_Documents/Asset List.xlsx
+++ b/Doorman_Documents/Asset List.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="219">
   <si>
     <t>flour</t>
     <phoneticPr fontId="5" type="noConversion"/>
@@ -745,6 +745,15 @@
   </si>
   <si>
     <t>DNA Splicer, Madam Feline's item</t>
+  </si>
+  <si>
+    <t>Bg_Lobby_Night.jpg</t>
+  </si>
+  <si>
+    <t>Lobby image for the night phase</t>
+  </si>
+  <si>
+    <t>1920 X1080</t>
   </si>
 </sst>
 </file>
@@ -1101,10 +1110,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0"/>
-  <dimension ref="A1:AC67"/>
+  <dimension ref="A1:AC68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1189,40 +1198,36 @@
       </c>
     </row>
     <row r="3" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="B3" t="s">
-        <v>156</v>
-      </c>
-      <c r="C3" t="s">
-        <v>157</v>
+      <c r="A3" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>217</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>150</v>
+        <v>218</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="G3" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="H3" s="9" t="s">
-        <v>47</v>
-      </c>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
     </row>
     <row r="4" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>145</v>
       </c>
       <c r="B4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>150</v>
@@ -1231,24 +1236,24 @@
         <v>151</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>152</v>
+        <v>189</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="H4" s="4" t="s">
-        <v>48</v>
+      <c r="H4" s="9" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>145</v>
       </c>
       <c r="B5" t="s">
-        <v>146</v>
+        <v>158</v>
       </c>
       <c r="C5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>150</v>
@@ -1257,13 +1262,13 @@
         <v>151</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>152</v>
+        <v>189</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>147</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1271,10 +1276,10 @@
         <v>145</v>
       </c>
       <c r="B6" t="s">
-        <v>161</v>
+        <v>146</v>
       </c>
       <c r="C6" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>150</v>
@@ -1283,13 +1288,13 @@
         <v>151</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>152</v>
+        <v>189</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>147</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1297,10 +1302,10 @@
         <v>145</v>
       </c>
       <c r="B7" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C7" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>150</v>
@@ -1315,7 +1320,7 @@
         <v>147</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1323,10 +1328,10 @@
         <v>145</v>
       </c>
       <c r="B8" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C8" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>150</v>
@@ -1335,39 +1340,39 @@
         <v>151</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>152</v>
+        <v>189</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>38</v>
+        <v>147</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>137</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>138</v>
+        <v>145</v>
+      </c>
+      <c r="B9" t="s">
+        <v>165</v>
+      </c>
+      <c r="C9" t="s">
+        <v>166</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>35</v>
+        <v>150</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>37</v>
+        <v>151</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>152</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>38</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1375,51 +1380,51 @@
         <v>136</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>59</v>
+        <v>137</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>54</v>
+        <v>138</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>35</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>55</v>
+        <v>36</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>189</v>
+        <v>37</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>38</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="B11" t="s">
-        <v>167</v>
-      </c>
-      <c r="C11" t="s">
-        <v>168</v>
+        <v>136</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>54</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>150</v>
+        <v>35</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>152</v>
+        <v>55</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>189</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>38</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1427,10 +1432,10 @@
         <v>145</v>
       </c>
       <c r="B12" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C12" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>150</v>
@@ -1445,59 +1450,59 @@
         <v>38</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>136</v>
+        <v>145</v>
       </c>
       <c r="B13" t="s">
-        <v>60</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>61</v>
+        <v>169</v>
+      </c>
+      <c r="C13" t="s">
+        <v>170</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>35</v>
+        <v>150</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>37</v>
+        <v>151</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>152</v>
       </c>
       <c r="G13" s="4" t="s">
         <v>38</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="B14" t="s">
-        <v>171</v>
-      </c>
-      <c r="C14" t="s">
-        <v>172</v>
+        <v>60</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>61</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>173</v>
+        <v>35</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>189</v>
+        <v>55</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1505,10 +1510,10 @@
         <v>145</v>
       </c>
       <c r="B15" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C15" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>173</v>
@@ -1523,7 +1528,7 @@
         <v>39</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1531,10 +1536,10 @@
         <v>145</v>
       </c>
       <c r="B16" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C16" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>173</v>
@@ -1549,7 +1554,7 @@
         <v>39</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1557,10 +1562,10 @@
         <v>145</v>
       </c>
       <c r="B17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C17" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>173</v>
@@ -1575,7 +1580,7 @@
         <v>39</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1583,10 +1588,10 @@
         <v>145</v>
       </c>
       <c r="B18" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C18" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>173</v>
@@ -1598,10 +1603,10 @@
         <v>189</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1609,10 +1614,10 @@
         <v>145</v>
       </c>
       <c r="B19" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C19" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>173</v>
@@ -1627,7 +1632,7 @@
         <v>40</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1635,10 +1640,10 @@
         <v>145</v>
       </c>
       <c r="B20" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C20" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>173</v>
@@ -1650,10 +1655,10 @@
         <v>189</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1661,25 +1666,25 @@
         <v>145</v>
       </c>
       <c r="B21" t="s">
-        <v>211</v>
+        <v>184</v>
       </c>
       <c r="C21" t="s">
-        <v>212</v>
+        <v>185</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>213</v>
+        <v>173</v>
       </c>
       <c r="E21" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="F21" s="2" t="s">
-        <v>152</v>
+      <c r="F21" s="1" t="s">
+        <v>189</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1687,13 +1692,13 @@
         <v>145</v>
       </c>
       <c r="B22" t="s">
-        <v>88</v>
+        <v>211</v>
       </c>
       <c r="C22" t="s">
-        <v>89</v>
+        <v>212</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>97</v>
+        <v>213</v>
       </c>
       <c r="E22" s="4" t="s">
         <v>151</v>
@@ -1705,7 +1710,7 @@
         <v>41</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1713,10 +1718,10 @@
         <v>145</v>
       </c>
       <c r="B23" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="C23" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>97</v>
@@ -1731,7 +1736,7 @@
         <v>41</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1739,10 +1744,10 @@
         <v>145</v>
       </c>
       <c r="B24" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C24" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D24" s="4" t="s">
         <v>97</v>
@@ -1757,7 +1762,7 @@
         <v>41</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1765,13 +1770,13 @@
         <v>145</v>
       </c>
       <c r="B25" t="s">
-        <v>214</v>
+        <v>100</v>
       </c>
       <c r="C25" t="s">
-        <v>215</v>
+        <v>101</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="E25" s="4" t="s">
         <v>151</v>
@@ -1783,7 +1788,7 @@
         <v>41</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1791,13 +1796,13 @@
         <v>145</v>
       </c>
       <c r="B26" t="s">
-        <v>75</v>
+        <v>214</v>
       </c>
       <c r="C26" t="s">
-        <v>76</v>
+        <v>215</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E26" s="4" t="s">
         <v>151</v>
@@ -1809,7 +1814,7 @@
         <v>41</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>0</v>
+        <v>71</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1817,13 +1822,13 @@
         <v>145</v>
       </c>
       <c r="B27" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C27" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E27" s="4" t="s">
         <v>151</v>
@@ -1832,10 +1837,10 @@
         <v>152</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1843,13 +1848,13 @@
         <v>145</v>
       </c>
       <c r="B28" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C28" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E28" s="4" t="s">
         <v>151</v>
@@ -1858,10 +1863,10 @@
         <v>152</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1869,13 +1874,13 @@
         <v>145</v>
       </c>
       <c r="B29" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C29" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E29" s="4" t="s">
         <v>151</v>
@@ -1884,10 +1889,10 @@
         <v>152</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1895,13 +1900,13 @@
         <v>145</v>
       </c>
       <c r="B30" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C30" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E30" s="4" t="s">
         <v>151</v>
@@ -1913,7 +1918,7 @@
         <v>41</v>
       </c>
       <c r="H30" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1921,13 +1926,13 @@
         <v>145</v>
       </c>
       <c r="B31" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C31" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E31" s="4" t="s">
         <v>151</v>
@@ -1939,7 +1944,7 @@
         <v>41</v>
       </c>
       <c r="H31" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1947,13 +1952,13 @@
         <v>145</v>
       </c>
       <c r="B32" t="s">
-        <v>115</v>
+        <v>85</v>
       </c>
       <c r="C32" t="s">
-        <v>116</v>
+        <v>86</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>119</v>
+        <v>96</v>
       </c>
       <c r="E32" s="4" t="s">
         <v>151</v>
@@ -1962,10 +1967,10 @@
         <v>152</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="H32" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1973,10 +1978,10 @@
         <v>145</v>
       </c>
       <c r="B33" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C33" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D33" s="4" t="s">
         <v>119</v>
@@ -1991,33 +1996,33 @@
         <v>34</v>
       </c>
       <c r="H33" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="B34" t="s">
+        <v>117</v>
+      </c>
+      <c r="C34" t="s">
+        <v>118</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="G34" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H34" s="4" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A34" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="B34" t="s">
-        <v>186</v>
-      </c>
-      <c r="C34" t="s">
-        <v>187</v>
-      </c>
-      <c r="D34" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="E34" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G34" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="H34" s="4" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
@@ -2025,13 +2030,13 @@
         <v>145</v>
       </c>
       <c r="B35" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C35" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="E35" s="4" t="s">
         <v>151</v>
@@ -2040,10 +2045,10 @@
         <v>189</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
@@ -2051,25 +2056,25 @@
         <v>145</v>
       </c>
       <c r="B36" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C36" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>150</v>
+        <v>192</v>
       </c>
       <c r="E36" s="4" t="s">
         <v>151</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>152</v>
+        <v>189</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="H36" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
@@ -2077,16 +2082,16 @@
         <v>145</v>
       </c>
       <c r="B37" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C37" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="D37" s="4" t="s">
         <v>150</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>102</v>
+        <v>151</v>
       </c>
       <c r="F37" s="1" t="s">
         <v>152</v>
@@ -2095,7 +2100,7 @@
         <v>34</v>
       </c>
       <c r="H37" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
@@ -2103,16 +2108,16 @@
         <v>145</v>
       </c>
       <c r="B38" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C38" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D38" s="4" t="s">
         <v>150</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>151</v>
+        <v>102</v>
       </c>
       <c r="F38" s="1" t="s">
         <v>152</v>
@@ -2121,7 +2126,7 @@
         <v>34</v>
       </c>
       <c r="H38" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
@@ -2129,16 +2134,16 @@
         <v>145</v>
       </c>
       <c r="B39" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C39" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D39" s="4" t="s">
         <v>150</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>102</v>
+        <v>151</v>
       </c>
       <c r="F39" s="1" t="s">
         <v>152</v>
@@ -2147,7 +2152,7 @@
         <v>34</v>
       </c>
       <c r="H39" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
@@ -2155,16 +2160,16 @@
         <v>145</v>
       </c>
       <c r="B40" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C40" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D40" s="4" t="s">
         <v>150</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>151</v>
+        <v>102</v>
       </c>
       <c r="F40" s="1" t="s">
         <v>152</v>
@@ -2173,50 +2178,50 @@
         <v>34</v>
       </c>
       <c r="H40" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="B41" s="8" t="s">
-        <v>133</v>
+        <v>145</v>
+      </c>
+      <c r="B41" t="s">
+        <v>201</v>
       </c>
       <c r="C41" t="s">
-        <v>203</v>
-      </c>
-      <c r="D41" s="7">
-        <v>0.13194444444444445</v>
-      </c>
-      <c r="E41" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="F41" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="G41" s="2" t="s">
-        <v>15</v>
+        <v>202</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="G41" s="4" t="s">
+        <v>34</v>
       </c>
       <c r="H41" s="4" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="B42" t="s">
-        <v>128</v>
+      <c r="B42" s="8" t="s">
+        <v>133</v>
       </c>
       <c r="C42" t="s">
-        <v>127</v>
+        <v>203</v>
       </c>
       <c r="D42" s="7">
-        <v>0.2388888888888889</v>
+        <v>0.13194444444444445</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="F42" s="6" t="s">
         <v>152</v>
@@ -2225,24 +2230,24 @@
         <v>15</v>
       </c>
       <c r="H42" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="B43" s="8" t="s">
-        <v>131</v>
+      <c r="B43" t="s">
+        <v>128</v>
       </c>
       <c r="C43" t="s">
-        <v>204</v>
+        <v>127</v>
       </c>
       <c r="D43" s="7">
-        <v>0.12291666666666667</v>
+        <v>0.2388888888888889</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F43" s="6" t="s">
         <v>152</v>
@@ -2251,7 +2256,7 @@
         <v>15</v>
       </c>
       <c r="H43" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
@@ -2259,16 +2264,16 @@
         <v>126</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C44" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D44" s="7">
-        <v>0.13333333333333333</v>
+        <v>0.12291666666666667</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="F44" s="6" t="s">
         <v>152</v>
@@ -2277,33 +2282,33 @@
         <v>15</v>
       </c>
       <c r="H44" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="B45" t="s">
-        <v>103</v>
+        <v>126</v>
+      </c>
+      <c r="B45" s="8" t="s">
+        <v>135</v>
       </c>
       <c r="C45" t="s">
-        <v>206</v>
-      </c>
-      <c r="D45" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="E45" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="F45" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="D45" s="7">
+        <v>0.13333333333333333</v>
+      </c>
+      <c r="E45" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="F45" s="6" t="s">
         <v>152</v>
       </c>
       <c r="G45" s="2" t="s">
         <v>15</v>
       </c>
       <c r="H45" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
@@ -2311,25 +2316,25 @@
         <v>148</v>
       </c>
       <c r="B46" t="s">
-        <v>124</v>
+        <v>103</v>
       </c>
       <c r="C46" t="s">
-        <v>207</v>
-      </c>
-      <c r="D46" t="s">
-        <v>120</v>
-      </c>
-      <c r="E46" t="s">
-        <v>121</v>
+        <v>206</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="E46" s="4" t="s">
+        <v>105</v>
       </c>
       <c r="F46" s="1" t="s">
         <v>152</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H46" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="47" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
@@ -2337,16 +2342,16 @@
         <v>148</v>
       </c>
       <c r="B47" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C47" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D47" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E47" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F47" s="1" t="s">
         <v>152</v>
@@ -2355,7 +2360,7 @@
         <v>16</v>
       </c>
       <c r="H47" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
@@ -2363,16 +2368,16 @@
         <v>148</v>
       </c>
       <c r="B48" t="s">
-        <v>109</v>
+        <v>125</v>
       </c>
       <c r="C48" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D48" t="s">
-        <v>111</v>
+        <v>122</v>
       </c>
       <c r="E48" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="F48" s="1" t="s">
         <v>152</v>
@@ -2381,7 +2386,7 @@
         <v>16</v>
       </c>
       <c r="H48" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="49" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
@@ -2389,25 +2394,25 @@
         <v>148</v>
       </c>
       <c r="B49" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C49" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D49" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E49" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="F49" s="1" t="s">
         <v>152</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H49" s="9" t="s">
-        <v>25</v>
+        <v>16</v>
+      </c>
+      <c r="H49" s="4" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="50" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
@@ -2415,55 +2420,78 @@
         <v>148</v>
       </c>
       <c r="B50" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="C50" t="s">
-        <v>87</v>
+        <v>210</v>
       </c>
       <c r="D50" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E50" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F50" s="1" t="s">
         <v>152</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H50" s="9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="51" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B51" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C51" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="D51" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="E51" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="F51" s="2" t="s">
-        <v>22</v>
+        <v>148</v>
+      </c>
+      <c r="B51" t="s">
+        <v>104</v>
+      </c>
+      <c r="C51" t="s">
+        <v>87</v>
+      </c>
+      <c r="D51" t="s">
+        <v>113</v>
+      </c>
+      <c r="E51" t="s">
+        <v>108</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>152</v>
       </c>
       <c r="G51" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H51" t="s">
+      <c r="H51" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A52" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B52" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C52" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D52" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E52" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F52" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G52" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H52" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="52" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="F52" s="1"/>
     </row>
     <row r="53" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="F53" s="1"/>
@@ -2509,6 +2537,9 @@
     </row>
     <row r="67" spans="6:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="F67" s="1"/>
+    </row>
+    <row r="68" spans="6:6" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F68" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>

</xml_diff>

<commit_message>
Finished Hall BG and Door pieces (door and doorframe). Deleted Image folder that was under the Game_Assets folder (to avoid confusion as to where to put the images).
Note: Bg_Door.png is now Bg_Door.jpg! File extension will need to be changed in the code.
</commit_message>
<xml_diff>
--- a/Doorman_Documents/Asset List.xlsx
+++ b/Doorman_Documents/Asset List.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="224">
   <si>
     <t>flour</t>
     <phoneticPr fontId="5" type="noConversion"/>
@@ -754,6 +754,21 @@
   </si>
   <si>
     <t>1920 X1080</t>
+  </si>
+  <si>
+    <t>Bg_Door.jpg</t>
+  </si>
+  <si>
+    <t>Door image for a hotel room</t>
+  </si>
+  <si>
+    <t>1134 X 1080</t>
+  </si>
+  <si>
+    <t>Bg_Doorframe.png</t>
+  </si>
+  <si>
+    <t>Door transparency/side walls.</t>
   </si>
 </sst>
 </file>
@@ -1110,10 +1125,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0"/>
-  <dimension ref="A1:AC68"/>
+  <dimension ref="A1:AC70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1314,7 +1329,7 @@
         <v>151</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>152</v>
+        <v>189</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>147</v>
@@ -1328,36 +1343,32 @@
         <v>145</v>
       </c>
       <c r="B8" t="s">
-        <v>163</v>
+        <v>219</v>
       </c>
       <c r="C8" t="s">
-        <v>164</v>
+        <v>220</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>150</v>
+        <v>221</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F8" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="G8" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>51</v>
-      </c>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
     </row>
     <row r="9" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>145</v>
       </c>
       <c r="B9" t="s">
-        <v>165</v>
+        <v>222</v>
       </c>
       <c r="C9" t="s">
-        <v>166</v>
+        <v>223</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>150</v>
@@ -1365,144 +1376,140 @@
       <c r="E9" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="F9" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>52</v>
-      </c>
+      <c r="F9" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
     </row>
     <row r="10" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>137</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>138</v>
+        <v>145</v>
+      </c>
+      <c r="B10" t="s">
+        <v>163</v>
+      </c>
+      <c r="C10" t="s">
+        <v>164</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>35</v>
+        <v>150</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>37</v>
+        <v>151</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>189</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>38</v>
+        <v>147</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>54</v>
+        <v>145</v>
+      </c>
+      <c r="B11" t="s">
+        <v>165</v>
+      </c>
+      <c r="C11" t="s">
+        <v>166</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>35</v>
+        <v>150</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>189</v>
+        <v>151</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>152</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>38</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="B12" t="s">
-        <v>167</v>
-      </c>
-      <c r="C12" t="s">
-        <v>168</v>
+        <v>136</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>138</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>150</v>
+        <v>35</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>152</v>
+        <v>36</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="G12" s="4" t="s">
         <v>38</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="B13" t="s">
-        <v>169</v>
-      </c>
-      <c r="C13" t="s">
-        <v>170</v>
+        <v>136</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>54</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>150</v>
+        <v>35</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>152</v>
+        <v>55</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>189</v>
       </c>
       <c r="G13" s="4" t="s">
         <v>38</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>136</v>
+        <v>145</v>
       </c>
       <c r="B14" t="s">
-        <v>60</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>61</v>
+        <v>167</v>
+      </c>
+      <c r="C14" t="s">
+        <v>168</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>35</v>
+        <v>150</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>37</v>
+        <v>151</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>152</v>
       </c>
       <c r="G14" s="4" t="s">
         <v>38</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1510,51 +1517,51 @@
         <v>145</v>
       </c>
       <c r="B15" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C15" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>173</v>
+        <v>150</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>151</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>189</v>
+        <v>152</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="B16" t="s">
-        <v>174</v>
-      </c>
-      <c r="C16" t="s">
-        <v>175</v>
+        <v>60</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>61</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>173</v>
+        <v>35</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>189</v>
+        <v>55</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1562,10 +1569,10 @@
         <v>145</v>
       </c>
       <c r="B17" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="C17" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>173</v>
@@ -1580,7 +1587,7 @@
         <v>39</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1588,10 +1595,10 @@
         <v>145</v>
       </c>
       <c r="B18" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="C18" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>173</v>
@@ -1606,7 +1613,7 @@
         <v>39</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1614,10 +1621,10 @@
         <v>145</v>
       </c>
       <c r="B19" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C19" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>173</v>
@@ -1629,10 +1636,10 @@
         <v>189</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1640,10 +1647,10 @@
         <v>145</v>
       </c>
       <c r="B20" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="C20" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>173</v>
@@ -1655,10 +1662,10 @@
         <v>189</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1666,10 +1673,10 @@
         <v>145</v>
       </c>
       <c r="B21" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="C21" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>173</v>
@@ -1681,10 +1688,10 @@
         <v>189</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1692,25 +1699,25 @@
         <v>145</v>
       </c>
       <c r="B22" t="s">
-        <v>211</v>
+        <v>182</v>
       </c>
       <c r="C22" t="s">
-        <v>212</v>
+        <v>183</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>213</v>
+        <v>173</v>
       </c>
       <c r="E22" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="F22" s="2" t="s">
-        <v>152</v>
+      <c r="F22" s="1" t="s">
+        <v>189</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1718,25 +1725,25 @@
         <v>145</v>
       </c>
       <c r="B23" t="s">
-        <v>88</v>
+        <v>184</v>
       </c>
       <c r="C23" t="s">
-        <v>89</v>
+        <v>185</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>97</v>
+        <v>173</v>
       </c>
       <c r="E23" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="F23" s="2" t="s">
-        <v>152</v>
+      <c r="F23" s="1" t="s">
+        <v>189</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1744,13 +1751,13 @@
         <v>145</v>
       </c>
       <c r="B24" t="s">
-        <v>98</v>
+        <v>211</v>
       </c>
       <c r="C24" t="s">
-        <v>99</v>
+        <v>212</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>97</v>
+        <v>213</v>
       </c>
       <c r="E24" s="4" t="s">
         <v>151</v>
@@ -1762,7 +1769,7 @@
         <v>41</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1770,10 +1777,10 @@
         <v>145</v>
       </c>
       <c r="B25" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="C25" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>97</v>
@@ -1788,7 +1795,7 @@
         <v>41</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1796,13 +1803,13 @@
         <v>145</v>
       </c>
       <c r="B26" t="s">
-        <v>214</v>
+        <v>98</v>
       </c>
       <c r="C26" t="s">
-        <v>215</v>
+        <v>99</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="E26" s="4" t="s">
         <v>151</v>
@@ -1814,7 +1821,7 @@
         <v>41</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1822,13 +1829,13 @@
         <v>145</v>
       </c>
       <c r="B27" t="s">
-        <v>75</v>
+        <v>100</v>
       </c>
       <c r="C27" t="s">
-        <v>76</v>
+        <v>101</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="E27" s="4" t="s">
         <v>151</v>
@@ -1840,7 +1847,7 @@
         <v>41</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>0</v>
+        <v>74</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1848,13 +1855,13 @@
         <v>145</v>
       </c>
       <c r="B28" t="s">
-        <v>77</v>
+        <v>214</v>
       </c>
       <c r="C28" t="s">
-        <v>78</v>
+        <v>215</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E28" s="4" t="s">
         <v>151</v>
@@ -1863,10 +1870,10 @@
         <v>152</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>1</v>
+        <v>71</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1874,13 +1881,13 @@
         <v>145</v>
       </c>
       <c r="B29" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C29" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E29" s="4" t="s">
         <v>151</v>
@@ -1889,10 +1896,10 @@
         <v>152</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1900,13 +1907,13 @@
         <v>145</v>
       </c>
       <c r="B30" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C30" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E30" s="4" t="s">
         <v>151</v>
@@ -1915,10 +1922,10 @@
         <v>152</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H30" s="4" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1926,13 +1933,13 @@
         <v>145</v>
       </c>
       <c r="B31" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C31" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E31" s="4" t="s">
         <v>151</v>
@@ -1941,10 +1948,10 @@
         <v>152</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="H31" s="4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1952,13 +1959,13 @@
         <v>145</v>
       </c>
       <c r="B32" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C32" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E32" s="4" t="s">
         <v>151</v>
@@ -1970,7 +1977,7 @@
         <v>41</v>
       </c>
       <c r="H32" s="4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1978,13 +1985,13 @@
         <v>145</v>
       </c>
       <c r="B33" t="s">
-        <v>115</v>
+        <v>83</v>
       </c>
       <c r="C33" t="s">
-        <v>116</v>
+        <v>84</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>119</v>
+        <v>95</v>
       </c>
       <c r="E33" s="4" t="s">
         <v>151</v>
@@ -1993,10 +2000,10 @@
         <v>152</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="H33" s="4" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2004,77 +2011,77 @@
         <v>145</v>
       </c>
       <c r="B34" t="s">
+        <v>85</v>
+      </c>
+      <c r="C34" t="s">
+        <v>86</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="G34" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="H34" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="B35" t="s">
+        <v>115</v>
+      </c>
+      <c r="C35" t="s">
+        <v>116</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="G35" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H35" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="B36" t="s">
         <v>117</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C36" t="s">
         <v>118</v>
       </c>
-      <c r="D34" s="4" t="s">
+      <c r="D36" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="E34" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="G34" s="4" t="s">
+      <c r="E36" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="G36" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="H34" s="4" t="s">
+      <c r="H36" s="4" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A35" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="B35" t="s">
-        <v>186</v>
-      </c>
-      <c r="C35" t="s">
-        <v>187</v>
-      </c>
-      <c r="D35" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="E35" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G35" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="H35" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A36" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="B36" t="s">
-        <v>190</v>
-      </c>
-      <c r="C36" t="s">
-        <v>191</v>
-      </c>
-      <c r="D36" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="E36" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G36" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="H36" s="4" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
@@ -2082,25 +2089,25 @@
         <v>145</v>
       </c>
       <c r="B37" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="C37" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>150</v>
+        <v>188</v>
       </c>
       <c r="E37" s="4" t="s">
         <v>151</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>152</v>
+        <v>189</v>
       </c>
       <c r="G37" s="4" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="H37" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
@@ -2108,25 +2115,25 @@
         <v>145</v>
       </c>
       <c r="B38" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="C38" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>150</v>
+        <v>192</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>102</v>
+        <v>151</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>152</v>
+        <v>189</v>
       </c>
       <c r="G38" s="4" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="H38" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
@@ -2134,10 +2141,10 @@
         <v>145</v>
       </c>
       <c r="B39" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C39" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="D39" s="4" t="s">
         <v>150</v>
@@ -2152,7 +2159,7 @@
         <v>34</v>
       </c>
       <c r="H39" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
@@ -2160,10 +2167,10 @@
         <v>145</v>
       </c>
       <c r="B40" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="C40" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="D40" s="4" t="s">
         <v>150</v>
@@ -2178,7 +2185,7 @@
         <v>34</v>
       </c>
       <c r="H40" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
@@ -2186,10 +2193,10 @@
         <v>145</v>
       </c>
       <c r="B41" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="C41" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="D41" s="4" t="s">
         <v>150</v>
@@ -2204,59 +2211,59 @@
         <v>34</v>
       </c>
       <c r="H41" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="B42" s="8" t="s">
-        <v>133</v>
+        <v>145</v>
+      </c>
+      <c r="B42" t="s">
+        <v>199</v>
       </c>
       <c r="C42" t="s">
-        <v>203</v>
-      </c>
-      <c r="D42" s="7">
-        <v>0.13194444444444445</v>
-      </c>
-      <c r="E42" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="F42" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="G42" s="2" t="s">
-        <v>15</v>
+        <v>200</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="G42" s="4" t="s">
+        <v>34</v>
       </c>
       <c r="H42" s="4" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>126</v>
+        <v>145</v>
       </c>
       <c r="B43" t="s">
-        <v>128</v>
+        <v>201</v>
       </c>
       <c r="C43" t="s">
-        <v>127</v>
-      </c>
-      <c r="D43" s="7">
-        <v>0.2388888888888889</v>
-      </c>
-      <c r="E43" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="F43" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="G43" s="2" t="s">
-        <v>15</v>
+        <v>202</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="E43" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="G43" s="4" t="s">
+        <v>34</v>
       </c>
       <c r="H43" s="4" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
@@ -2264,16 +2271,16 @@
         <v>126</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C44" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D44" s="7">
-        <v>0.12291666666666667</v>
+        <v>0.13194444444444445</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="F44" s="6" t="s">
         <v>152</v>
@@ -2282,24 +2289,24 @@
         <v>15</v>
       </c>
       <c r="H44" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="B45" s="8" t="s">
-        <v>135</v>
+      <c r="B45" t="s">
+        <v>128</v>
       </c>
       <c r="C45" t="s">
-        <v>205</v>
+        <v>127</v>
       </c>
       <c r="D45" s="7">
-        <v>0.13333333333333333</v>
+        <v>0.2388888888888889</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="F45" s="6" t="s">
         <v>152</v>
@@ -2308,59 +2315,59 @@
         <v>15</v>
       </c>
       <c r="H45" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="B46" t="s">
-        <v>103</v>
+        <v>126</v>
+      </c>
+      <c r="B46" s="8" t="s">
+        <v>131</v>
       </c>
       <c r="C46" t="s">
-        <v>206</v>
-      </c>
-      <c r="D46" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="E46" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="F46" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="D46" s="7">
+        <v>0.12291666666666667</v>
+      </c>
+      <c r="E46" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="F46" s="6" t="s">
         <v>152</v>
       </c>
       <c r="G46" s="2" t="s">
         <v>15</v>
       </c>
       <c r="H46" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="47" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="B47" t="s">
-        <v>124</v>
+        <v>126</v>
+      </c>
+      <c r="B47" s="8" t="s">
+        <v>135</v>
       </c>
       <c r="C47" t="s">
-        <v>207</v>
-      </c>
-      <c r="D47" t="s">
-        <v>120</v>
-      </c>
-      <c r="E47" t="s">
-        <v>121</v>
-      </c>
-      <c r="F47" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="D47" s="7">
+        <v>0.13333333333333333</v>
+      </c>
+      <c r="E47" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="F47" s="6" t="s">
         <v>152</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H47" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
@@ -2368,25 +2375,25 @@
         <v>148</v>
       </c>
       <c r="B48" t="s">
-        <v>125</v>
+        <v>103</v>
       </c>
       <c r="C48" t="s">
-        <v>208</v>
-      </c>
-      <c r="D48" t="s">
-        <v>122</v>
-      </c>
-      <c r="E48" t="s">
-        <v>123</v>
+        <v>206</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="E48" s="4" t="s">
+        <v>105</v>
       </c>
       <c r="F48" s="1" t="s">
         <v>152</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H48" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="49" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
@@ -2394,16 +2401,16 @@
         <v>148</v>
       </c>
       <c r="B49" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
       <c r="C49" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D49" t="s">
-        <v>111</v>
+        <v>120</v>
       </c>
       <c r="E49" t="s">
-        <v>110</v>
+        <v>121</v>
       </c>
       <c r="F49" s="1" t="s">
         <v>152</v>
@@ -2412,7 +2419,7 @@
         <v>16</v>
       </c>
       <c r="H49" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="50" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
@@ -2420,25 +2427,25 @@
         <v>148</v>
       </c>
       <c r="B50" t="s">
-        <v>107</v>
+        <v>125</v>
       </c>
       <c r="C50" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D50" t="s">
-        <v>112</v>
+        <v>122</v>
       </c>
       <c r="E50" t="s">
-        <v>106</v>
+        <v>123</v>
       </c>
       <c r="F50" s="1" t="s">
         <v>152</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H50" s="9" t="s">
-        <v>25</v>
+        <v>16</v>
+      </c>
+      <c r="H50" s="4" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="51" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
@@ -2446,16 +2453,16 @@
         <v>148</v>
       </c>
       <c r="B51" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="C51" t="s">
-        <v>87</v>
+        <v>209</v>
       </c>
       <c r="D51" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E51" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="F51" s="1" t="s">
         <v>152</v>
@@ -2463,41 +2470,87 @@
       <c r="G51" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H51" s="9" t="s">
-        <v>24</v>
+      <c r="H51" s="4" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="52" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="B52" t="s">
+        <v>107</v>
+      </c>
+      <c r="C52" t="s">
+        <v>210</v>
+      </c>
+      <c r="D52" t="s">
+        <v>112</v>
+      </c>
+      <c r="E52" t="s">
+        <v>106</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="G52" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H52" s="9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A53" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="B53" t="s">
+        <v>104</v>
+      </c>
+      <c r="C53" t="s">
+        <v>87</v>
+      </c>
+      <c r="D53" t="s">
+        <v>113</v>
+      </c>
+      <c r="E53" t="s">
+        <v>108</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="G53" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H53" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A54" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B52" s="9" t="s">
+      <c r="B54" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C52" s="9" t="s">
+      <c r="C54" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="D52" s="9" t="s">
+      <c r="D54" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="E52" s="8" t="s">
+      <c r="E54" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="F52" s="2" t="s">
+      <c r="F54" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G52" s="2" t="s">
+      <c r="G54" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H52" t="s">
+      <c r="H54" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="53" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="F53" s="1"/>
-    </row>
-    <row r="54" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="F54" s="1"/>
     </row>
     <row r="55" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="F55" s="1"/>
@@ -2540,6 +2593,12 @@
     </row>
     <row r="68" spans="6:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="F68" s="1"/>
+    </row>
+    <row r="69" spans="6:6" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F69" s="1"/>
+    </row>
+    <row r="70" spans="6:6" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F70" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>

</xml_diff>

<commit_message>
Menu image (still under Bg_Menu.jpg).
</commit_message>
<xml_diff>
--- a/Doorman_Documents/Asset List.xlsx
+++ b/Doorman_Documents/Asset List.xlsx
@@ -1127,8 +1127,8 @@
   <sheetPr published="0"/>
   <dimension ref="A1:AC70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G47" sqref="G47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2153,7 +2153,7 @@
         <v>151</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>152</v>
+        <v>189</v>
       </c>
       <c r="G39" s="4" t="s">
         <v>34</v>

</xml_diff>

<commit_message>
Added check image, updated asset list.
</commit_message>
<xml_diff>
--- a/Doorman_Documents/Asset List.xlsx
+++ b/Doorman_Documents/Asset List.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="226">
   <si>
     <t>flour</t>
     <phoneticPr fontId="5" type="noConversion"/>
@@ -168,10 +168,6 @@
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>copy of Kyles image</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
     <t>Placeholder</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
@@ -769,6 +765,15 @@
   </si>
   <si>
     <t>Door transparency/side walls.</t>
+  </si>
+  <si>
+    <t>Item_Check.png</t>
+  </si>
+  <si>
+    <t>Check for story sequence</t>
+  </si>
+  <si>
+    <t>1143 X 720</t>
   </si>
 </sst>
 </file>
@@ -1125,10 +1130,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0"/>
-  <dimension ref="A1:AC70"/>
+  <dimension ref="A1:AC71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G47" sqref="G47"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1141,28 +1146,28 @@
   <sheetData>
     <row r="1" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>143</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>144</v>
       </c>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
@@ -1188,1372 +1193,1391 @@
     </row>
     <row r="2" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>155</v>
-      </c>
       <c r="D2" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>216</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" s="4" t="s">
         <v>217</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>218</v>
-      </c>
       <c r="E3" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
     </row>
     <row r="4" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B4" t="s">
+        <v>155</v>
+      </c>
+      <c r="C4" t="s">
         <v>156</v>
       </c>
-      <c r="C4" t="s">
-        <v>157</v>
-      </c>
       <c r="D4" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B5" t="s">
+        <v>157</v>
+      </c>
+      <c r="C5" t="s">
         <v>158</v>
       </c>
-      <c r="C5" t="s">
-        <v>159</v>
-      </c>
       <c r="D5" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="B6" t="s">
         <v>145</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
+        <v>159</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="G6" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="C6" t="s">
-        <v>160</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>147</v>
-      </c>
       <c r="H6" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B7" t="s">
+        <v>160</v>
+      </c>
+      <c r="C7" t="s">
         <v>161</v>
       </c>
-      <c r="C7" t="s">
-        <v>162</v>
-      </c>
       <c r="D7" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B8" t="s">
+        <v>218</v>
+      </c>
+      <c r="C8" t="s">
         <v>219</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" s="4" t="s">
         <v>220</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>221</v>
-      </c>
       <c r="E8" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
     </row>
     <row r="9" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B9" t="s">
+        <v>221</v>
+      </c>
+      <c r="C9" t="s">
         <v>222</v>
       </c>
-      <c r="C9" t="s">
-        <v>223</v>
-      </c>
       <c r="D9" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
     </row>
     <row r="10" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B10" t="s">
+        <v>162</v>
+      </c>
+      <c r="C10" t="s">
         <v>163</v>
       </c>
-      <c r="C10" t="s">
-        <v>164</v>
-      </c>
       <c r="D10" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B11" t="s">
+        <v>164</v>
+      </c>
+      <c r="C11" t="s">
         <v>165</v>
       </c>
-      <c r="C11" t="s">
-        <v>166</v>
-      </c>
       <c r="D11" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>152</v>
+        <v>188</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="B12" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="C12" s="9" t="s">
         <v>137</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>138</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>35</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>36</v>
+        <v>150</v>
       </c>
       <c r="F12" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="G12" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="G12" s="4" t="s">
-        <v>38</v>
-      </c>
       <c r="H12" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>35</v>
       </c>
       <c r="E13" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H13" s="4" t="s">
         <v>55</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B14" t="s">
+        <v>166</v>
+      </c>
+      <c r="C14" t="s">
         <v>167</v>
       </c>
-      <c r="C14" t="s">
-        <v>168</v>
-      </c>
       <c r="D14" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B15" t="s">
+        <v>168</v>
+      </c>
+      <c r="C15" t="s">
         <v>169</v>
       </c>
-      <c r="C15" t="s">
-        <v>170</v>
-      </c>
       <c r="D15" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B16" t="s">
+        <v>59</v>
+      </c>
+      <c r="C16" s="9" t="s">
         <v>60</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>61</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>35</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F16" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G16" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="G16" s="4" t="s">
-        <v>38</v>
-      </c>
       <c r="H16" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B17" t="s">
+        <v>170</v>
+      </c>
+      <c r="C17" t="s">
         <v>171</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="D17" s="4" t="s">
-        <v>173</v>
-      </c>
       <c r="E17" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B18" t="s">
+        <v>173</v>
+      </c>
+      <c r="C18" t="s">
         <v>174</v>
       </c>
-      <c r="C18" t="s">
-        <v>175</v>
-      </c>
       <c r="D18" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B19" t="s">
+        <v>175</v>
+      </c>
+      <c r="C19" t="s">
         <v>176</v>
       </c>
-      <c r="C19" t="s">
-        <v>177</v>
-      </c>
       <c r="D19" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B20" t="s">
+        <v>177</v>
+      </c>
+      <c r="C20" t="s">
         <v>178</v>
       </c>
-      <c r="C20" t="s">
-        <v>179</v>
-      </c>
       <c r="D20" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B21" t="s">
+        <v>179</v>
+      </c>
+      <c r="C21" t="s">
         <v>180</v>
       </c>
-      <c r="C21" t="s">
-        <v>181</v>
-      </c>
       <c r="D21" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B22" t="s">
+        <v>181</v>
+      </c>
+      <c r="C22" t="s">
         <v>182</v>
       </c>
-      <c r="C22" t="s">
-        <v>183</v>
-      </c>
       <c r="D22" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B23" t="s">
+        <v>183</v>
+      </c>
+      <c r="C23" t="s">
         <v>184</v>
       </c>
-      <c r="C23" t="s">
-        <v>185</v>
-      </c>
       <c r="D23" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B24" t="s">
-        <v>211</v>
+        <v>223</v>
       </c>
       <c r="C24" t="s">
-        <v>212</v>
+        <v>224</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>213</v>
+        <v>225</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="G24" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="H24" s="4" t="s">
-        <v>70</v>
-      </c>
+        <v>188</v>
+      </c>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
     </row>
     <row r="25" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B25" t="s">
-        <v>88</v>
+        <v>210</v>
       </c>
       <c r="C25" t="s">
-        <v>89</v>
+        <v>211</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>97</v>
+        <v>212</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B26" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="C26" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B27" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C27" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B28" t="s">
-        <v>214</v>
+        <v>99</v>
       </c>
       <c r="C28" t="s">
-        <v>215</v>
+        <v>100</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B29" t="s">
-        <v>75</v>
+        <v>213</v>
       </c>
       <c r="C29" t="s">
-        <v>76</v>
+        <v>214</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>0</v>
+        <v>70</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B30" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C30" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H30" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B31" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C31" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H31" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B32" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C32" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H32" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B33" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C33" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H33" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B34" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C34" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H34" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B35" t="s">
-        <v>115</v>
+        <v>84</v>
       </c>
       <c r="C35" t="s">
-        <v>116</v>
+        <v>85</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>119</v>
+        <v>95</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B36" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C36" t="s">
+        <v>115</v>
+      </c>
+      <c r="D36" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="D36" s="4" t="s">
-        <v>119</v>
-      </c>
       <c r="E36" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G36" s="4" t="s">
         <v>34</v>
       </c>
       <c r="H36" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="B37" t="s">
+        <v>116</v>
+      </c>
+      <c r="C37" t="s">
+        <v>117</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="G37" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H37" s="4" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A37" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="B37" t="s">
-        <v>186</v>
-      </c>
-      <c r="C37" t="s">
-        <v>187</v>
-      </c>
-      <c r="D37" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="E37" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G37" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="H37" s="4" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B38" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="C38" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G38" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H38" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B39" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="C39" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>150</v>
+        <v>191</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G39" s="4" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="H39" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B40" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C40" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>102</v>
+        <v>150</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>152</v>
+        <v>188</v>
       </c>
       <c r="G40" s="4" t="s">
         <v>34</v>
       </c>
       <c r="H40" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B41" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C41" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>151</v>
+        <v>101</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G41" s="4" t="s">
         <v>34</v>
       </c>
       <c r="H41" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B42" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C42" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>102</v>
+        <v>150</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G42" s="4" t="s">
         <v>34</v>
       </c>
       <c r="H42" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B43" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="C43" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>151</v>
+        <v>101</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G43" s="4" t="s">
         <v>34</v>
       </c>
       <c r="H43" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="B44" s="8" t="s">
-        <v>133</v>
+        <v>144</v>
+      </c>
+      <c r="B44" t="s">
+        <v>200</v>
       </c>
       <c r="C44" t="s">
-        <v>203</v>
-      </c>
-      <c r="D44" s="7">
-        <v>0.13194444444444445</v>
-      </c>
-      <c r="E44" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="F44" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="G44" s="2" t="s">
-        <v>15</v>
+        <v>201</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="G44" s="4" t="s">
+        <v>34</v>
       </c>
       <c r="H44" s="4" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="B45" t="s">
-        <v>128</v>
+        <v>125</v>
+      </c>
+      <c r="B45" s="8" t="s">
+        <v>132</v>
       </c>
       <c r="C45" t="s">
-        <v>127</v>
+        <v>202</v>
       </c>
       <c r="D45" s="7">
-        <v>0.2388888888888889</v>
+        <v>0.13194444444444445</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="F45" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G45" s="2" t="s">
         <v>15</v>
       </c>
       <c r="H45" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="B46" t="s">
+        <v>127</v>
+      </c>
+      <c r="C46" t="s">
         <v>126</v>
       </c>
-      <c r="B46" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="C46" t="s">
-        <v>204</v>
-      </c>
       <c r="D46" s="7">
-        <v>0.12291666666666667</v>
+        <v>0.2388888888888889</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F46" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G46" s="2" t="s">
         <v>15</v>
       </c>
       <c r="H46" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="47" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="C47" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D47" s="7">
-        <v>0.13333333333333333</v>
+        <v>0.12291666666666667</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="F47" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G47" s="2" t="s">
         <v>15</v>
       </c>
       <c r="H47" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="B48" t="s">
-        <v>103</v>
+        <v>125</v>
+      </c>
+      <c r="B48" s="8" t="s">
+        <v>134</v>
       </c>
       <c r="C48" t="s">
-        <v>206</v>
-      </c>
-      <c r="D48" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="E48" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="F48" s="1" t="s">
-        <v>152</v>
+        <v>204</v>
+      </c>
+      <c r="D48" s="7">
+        <v>0.13333333333333333</v>
+      </c>
+      <c r="E48" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="F48" s="6" t="s">
+        <v>151</v>
       </c>
       <c r="G48" s="2" t="s">
         <v>15</v>
       </c>
       <c r="H48" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="49" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B49" t="s">
-        <v>124</v>
+        <v>102</v>
       </c>
       <c r="C49" t="s">
-        <v>207</v>
-      </c>
-      <c r="D49" t="s">
-        <v>120</v>
-      </c>
-      <c r="E49" t="s">
-        <v>121</v>
+        <v>205</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="E49" s="4" t="s">
+        <v>104</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H49" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="50" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B50" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C50" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D50" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E50" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G50" s="2" t="s">
         <v>16</v>
       </c>
       <c r="H50" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="51" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B51" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
       <c r="C51" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D51" t="s">
-        <v>111</v>
+        <v>121</v>
       </c>
       <c r="E51" t="s">
-        <v>110</v>
+        <v>122</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G51" s="2" t="s">
         <v>16</v>
       </c>
       <c r="H51" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="52" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B52" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C52" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D52" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E52" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H52" s="9" t="s">
-        <v>25</v>
+        <v>16</v>
+      </c>
+      <c r="H52" s="4" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="53" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B53" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C53" t="s">
-        <v>87</v>
+        <v>209</v>
       </c>
       <c r="D53" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E53" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G53" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H53" s="9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="54" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B54" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C54" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="D54" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="E54" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="F54" s="2" t="s">
-        <v>22</v>
+        <v>147</v>
+      </c>
+      <c r="B54" t="s">
+        <v>103</v>
+      </c>
+      <c r="C54" t="s">
+        <v>86</v>
+      </c>
+      <c r="D54" t="s">
+        <v>112</v>
+      </c>
+      <c r="E54" t="s">
+        <v>107</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>151</v>
       </c>
       <c r="G54" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H54" t="s">
+      <c r="H54" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A55" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B55" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C55" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D55" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E55" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F55" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G55" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H55" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="55" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="F55" s="1"/>
     </row>
     <row r="56" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="F56" s="1"/>
@@ -2599,6 +2623,9 @@
     </row>
     <row r="70" spans="6:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="F70" s="1"/>
+    </row>
+    <row r="71" spans="6:6" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F71" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>

</xml_diff>

<commit_message>
Promo image, a couple of items done.
</commit_message>
<xml_diff>
--- a/Doorman_Documents/Asset List.xlsx
+++ b/Doorman_Documents/Asset List.xlsx
@@ -24,235 +24,235 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="227">
   <si>
     <t>flour</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>fleece</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>football</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>watch</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>heel</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>candle</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>textWin</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>textLose</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>logo</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>icon</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>bgMenu</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>bgOptions</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>bgDifficulty</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>gameMenu</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>credits</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>na</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>na</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">sound </t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>snore.mp3</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">Snore sound for </t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>3.0 sec</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>Hollywood sound effects library</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>Final</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>sound_snore</t>
   </si>
   <si>
     <t>sound_ring</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>sound_door</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>music_menu</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>music_intro</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>music_lobby</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>music_night</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>sound_ding</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>music_lose</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>music_win</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>sound_click</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>mnu</t>
   </si>
   <si>
     <t>1920 X 1080</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>Placeholder</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>bg</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>char</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>char</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>item</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>item</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>item</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>logo</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>logo</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>lobby</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>lobbyBlur</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>elevator</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>buttons</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>hall</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>room</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>jimRoom</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>jimRoomNight</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>A completely black screen representing jims eyes</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>image by Baiey</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>night</t>
   </si>
   <si>
     <t>jail</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>shop</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>Bg_Night.png</t>
@@ -262,59 +262,59 @@
   </si>
   <si>
     <t>The town in the game, camera scrolls past</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>town</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>chris</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>coach</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>colonel</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>edmond</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>jason</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>kim</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>madam</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>phone</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>splicer</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>clock</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>minute</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>hour</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>Item_Flour.png</t>
@@ -501,15 +501,15 @@
   </si>
   <si>
     <t>image</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>Bg_Jimroom_Night.jpg</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>Jim's room at night</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>Type</t>
@@ -774,13 +774,16 @@
   </si>
   <si>
     <t>1143 X 720</t>
+  </si>
+  <si>
+    <t>Final</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -799,10 +802,6 @@
     <font>
       <sz val="10"/>
       <color indexed="8"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -830,7 +829,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -841,9 +840,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="20" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1132,8 +1128,8 @@
   <sheetPr published="0"/>
   <dimension ref="A1:AC71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="E56" sqref="E56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1261,7 +1257,7 @@
       <c r="G4" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="H4" s="9" t="s">
+      <c r="H4" s="8" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1443,10 +1439,10 @@
       <c r="A12" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="8" t="s">
         <v>137</v>
       </c>
       <c r="D12" s="4" t="s">
@@ -1469,10 +1465,10 @@
       <c r="A13" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="8" t="s">
         <v>53</v>
       </c>
       <c r="D13" s="4" t="s">
@@ -1508,7 +1504,7 @@
         <v>150</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>151</v>
+        <v>188</v>
       </c>
       <c r="G14" s="4" t="s">
         <v>37</v>
@@ -1534,7 +1530,7 @@
         <v>150</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>151</v>
+        <v>188</v>
       </c>
       <c r="G15" s="4" t="s">
         <v>37</v>
@@ -1550,7 +1546,7 @@
       <c r="B16" t="s">
         <v>59</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="C16" s="8" t="s">
         <v>60</v>
       </c>
       <c r="D16" s="4" t="s">
@@ -2297,20 +2293,20 @@
       <c r="A45" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="B45" s="8" t="s">
+      <c r="B45" s="7" t="s">
         <v>132</v>
       </c>
       <c r="C45" t="s">
         <v>202</v>
       </c>
-      <c r="D45" s="7">
+      <c r="D45" s="6">
         <v>0.13194444444444445</v>
       </c>
       <c r="E45" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="F45" s="6" t="s">
-        <v>151</v>
+      <c r="F45" s="2" t="s">
+        <v>226</v>
       </c>
       <c r="G45" s="2" t="s">
         <v>15</v>
@@ -2329,14 +2325,14 @@
       <c r="C46" t="s">
         <v>126</v>
       </c>
-      <c r="D46" s="7">
+      <c r="D46" s="6">
         <v>0.2388888888888889</v>
       </c>
       <c r="E46" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="F46" s="6" t="s">
-        <v>151</v>
+      <c r="F46" s="2" t="s">
+        <v>226</v>
       </c>
       <c r="G46" s="2" t="s">
         <v>15</v>
@@ -2349,20 +2345,20 @@
       <c r="A47" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="B47" s="8" t="s">
+      <c r="B47" s="7" t="s">
         <v>130</v>
       </c>
       <c r="C47" t="s">
         <v>203</v>
       </c>
-      <c r="D47" s="7">
+      <c r="D47" s="6">
         <v>0.12291666666666667</v>
       </c>
       <c r="E47" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="F47" s="6" t="s">
-        <v>151</v>
+      <c r="F47" s="2" t="s">
+        <v>226</v>
       </c>
       <c r="G47" s="2" t="s">
         <v>15</v>
@@ -2375,20 +2371,20 @@
       <c r="A48" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="B48" s="8" t="s">
+      <c r="B48" s="7" t="s">
         <v>134</v>
       </c>
       <c r="C48" t="s">
         <v>204</v>
       </c>
-      <c r="D48" s="7">
+      <c r="D48" s="6">
         <v>0.13333333333333333</v>
       </c>
       <c r="E48" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="F48" s="6" t="s">
-        <v>151</v>
+      <c r="F48" s="2" t="s">
+        <v>226</v>
       </c>
       <c r="G48" s="2" t="s">
         <v>15</v>
@@ -2414,7 +2410,7 @@
         <v>104</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>151</v>
+        <v>226</v>
       </c>
       <c r="G49" s="2" t="s">
         <v>15</v>
@@ -2440,7 +2436,7 @@
         <v>120</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>151</v>
+        <v>226</v>
       </c>
       <c r="G50" s="2" t="s">
         <v>16</v>
@@ -2466,7 +2462,7 @@
         <v>122</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>151</v>
+        <v>226</v>
       </c>
       <c r="G51" s="2" t="s">
         <v>16</v>
@@ -2492,7 +2488,7 @@
         <v>109</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>151</v>
+        <v>226</v>
       </c>
       <c r="G52" s="2" t="s">
         <v>16</v>
@@ -2518,12 +2514,12 @@
         <v>105</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>151</v>
+        <v>226</v>
       </c>
       <c r="G53" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H53" s="9" t="s">
+      <c r="H53" s="8" t="s">
         <v>25</v>
       </c>
     </row>
@@ -2544,12 +2540,12 @@
         <v>107</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>151</v>
+        <v>226</v>
       </c>
       <c r="G54" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H54" s="9" t="s">
+      <c r="H54" s="8" t="s">
         <v>24</v>
       </c>
     </row>
@@ -2557,16 +2553,16 @@
       <c r="A55" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B55" s="9" t="s">
+      <c r="B55" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C55" s="9" t="s">
+      <c r="C55" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D55" s="9" t="s">
+      <c r="D55" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="E55" s="8" t="s">
+      <c r="E55" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F55" s="2" t="s">
@@ -2628,7 +2624,7 @@
       <c r="F71" s="1"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="5" type="noConversion"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293"/>
   <extLst>

</xml_diff>

<commit_message>
Clock is now 10% better.
</commit_message>
<xml_diff>
--- a/Doorman_Documents/Asset List.xlsx
+++ b/Doorman_Documents/Asset List.xlsx
@@ -258,9 +258,6 @@
     <t>Bg_Night.png</t>
   </si>
   <si>
-    <t>Bg_Town.png</t>
-  </si>
-  <si>
     <t>The town in the game, camera scrolls past</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
@@ -777,6 +774,9 @@
   </si>
   <si>
     <t>Final</t>
+  </si>
+  <si>
+    <t>Bg_City.jpg</t>
   </si>
 </sst>
 </file>
@@ -1128,8 +1128,8 @@
   <sheetPr published="0"/>
   <dimension ref="A1:AC71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="E56" sqref="E56"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1142,28 +1142,28 @@
   <sheetData>
     <row r="1" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>142</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>143</v>
       </c>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
@@ -1189,25 +1189,25 @@
     </row>
     <row r="2" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>154</v>
-      </c>
       <c r="D2" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>45</v>
@@ -1215,47 +1215,47 @@
     </row>
     <row r="3" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>215</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" s="4" t="s">
         <v>216</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>217</v>
-      </c>
       <c r="E3" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
     </row>
     <row r="4" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B4" t="s">
+        <v>154</v>
+      </c>
+      <c r="C4" t="s">
         <v>155</v>
       </c>
-      <c r="C4" t="s">
-        <v>156</v>
-      </c>
       <c r="D4" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H4" s="8" t="s">
         <v>46</v>
@@ -1263,25 +1263,25 @@
     </row>
     <row r="5" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B5" t="s">
+        <v>156</v>
+      </c>
+      <c r="C5" t="s">
         <v>157</v>
       </c>
-      <c r="C5" t="s">
-        <v>158</v>
-      </c>
       <c r="D5" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H5" s="4" t="s">
         <v>47</v>
@@ -1289,25 +1289,25 @@
     </row>
     <row r="6" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="B6" t="s">
         <v>144</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
+        <v>158</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="G6" s="4" t="s">
         <v>145</v>
-      </c>
-      <c r="C6" t="s">
-        <v>159</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>146</v>
       </c>
       <c r="H6" s="4" t="s">
         <v>48</v>
@@ -1315,25 +1315,25 @@
     </row>
     <row r="7" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B7" t="s">
+        <v>159</v>
+      </c>
+      <c r="C7" t="s">
         <v>160</v>
       </c>
-      <c r="C7" t="s">
-        <v>161</v>
-      </c>
       <c r="D7" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H7" s="4" t="s">
         <v>49</v>
@@ -1341,69 +1341,69 @@
     </row>
     <row r="8" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B8" t="s">
+        <v>217</v>
+      </c>
+      <c r="C8" t="s">
         <v>218</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" s="4" t="s">
         <v>219</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>220</v>
-      </c>
       <c r="E8" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
     </row>
     <row r="9" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B9" t="s">
+        <v>220</v>
+      </c>
+      <c r="C9" t="s">
         <v>221</v>
       </c>
-      <c r="C9" t="s">
-        <v>222</v>
-      </c>
       <c r="D9" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
     </row>
     <row r="10" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B10" t="s">
+        <v>161</v>
+      </c>
+      <c r="C10" t="s">
         <v>162</v>
       </c>
-      <c r="C10" t="s">
-        <v>163</v>
-      </c>
       <c r="D10" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H10" s="4" t="s">
         <v>50</v>
@@ -1411,22 +1411,22 @@
     </row>
     <row r="11" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B11" t="s">
+        <v>163</v>
+      </c>
+      <c r="C11" t="s">
         <v>164</v>
       </c>
-      <c r="C11" t="s">
-        <v>165</v>
-      </c>
       <c r="D11" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>37</v>
@@ -1437,22 +1437,22 @@
     </row>
     <row r="12" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="B12" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="C12" s="8" t="s">
         <v>136</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>137</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>35</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G12" s="4" t="s">
         <v>37</v>
@@ -1463,7 +1463,7 @@
     </row>
     <row r="13" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B13" s="8" t="s">
         <v>58</v>
@@ -1478,7 +1478,7 @@
         <v>54</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G13" s="4" t="s">
         <v>37</v>
@@ -1489,22 +1489,22 @@
     </row>
     <row r="14" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B14" t="s">
+        <v>165</v>
+      </c>
+      <c r="C14" t="s">
         <v>166</v>
       </c>
-      <c r="C14" t="s">
-        <v>167</v>
-      </c>
       <c r="D14" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G14" s="4" t="s">
         <v>37</v>
@@ -1515,22 +1515,22 @@
     </row>
     <row r="15" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B15" t="s">
+        <v>167</v>
+      </c>
+      <c r="C15" t="s">
         <v>168</v>
       </c>
-      <c r="C15" t="s">
-        <v>169</v>
-      </c>
       <c r="D15" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G15" s="4" t="s">
         <v>37</v>
@@ -1541,19 +1541,19 @@
     </row>
     <row r="16" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B16" t="s">
+        <v>226</v>
+      </c>
+      <c r="C16" s="8" t="s">
         <v>59</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>60</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>35</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>54</v>
+        <v>149</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>36</v>
@@ -1562,361 +1562,361 @@
         <v>37</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B17" t="s">
+        <v>169</v>
+      </c>
+      <c r="C17" t="s">
         <v>170</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="D17" s="4" t="s">
-        <v>172</v>
-      </c>
       <c r="E17" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G17" s="4" t="s">
         <v>38</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B18" t="s">
+        <v>172</v>
+      </c>
+      <c r="C18" t="s">
         <v>173</v>
       </c>
-      <c r="C18" t="s">
-        <v>174</v>
-      </c>
       <c r="D18" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G18" s="4" t="s">
         <v>38</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B19" t="s">
+        <v>174</v>
+      </c>
+      <c r="C19" t="s">
         <v>175</v>
       </c>
-      <c r="C19" t="s">
-        <v>176</v>
-      </c>
       <c r="D19" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G19" s="4" t="s">
         <v>38</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B20" t="s">
+        <v>176</v>
+      </c>
+      <c r="C20" t="s">
         <v>177</v>
       </c>
-      <c r="C20" t="s">
-        <v>178</v>
-      </c>
       <c r="D20" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G20" s="4" t="s">
         <v>38</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B21" t="s">
+        <v>178</v>
+      </c>
+      <c r="C21" t="s">
         <v>179</v>
       </c>
-      <c r="C21" t="s">
-        <v>180</v>
-      </c>
       <c r="D21" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G21" s="4" t="s">
         <v>39</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B22" t="s">
+        <v>180</v>
+      </c>
+      <c r="C22" t="s">
         <v>181</v>
       </c>
-      <c r="C22" t="s">
-        <v>182</v>
-      </c>
       <c r="D22" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G22" s="4" t="s">
         <v>39</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B23" t="s">
+        <v>182</v>
+      </c>
+      <c r="C23" t="s">
         <v>183</v>
       </c>
-      <c r="C23" t="s">
-        <v>184</v>
-      </c>
       <c r="D23" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G23" s="4" t="s">
         <v>38</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B24" t="s">
+        <v>222</v>
+      </c>
+      <c r="C24" t="s">
         <v>223</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" s="4" t="s">
         <v>224</v>
       </c>
-      <c r="D24" s="4" t="s">
-        <v>225</v>
-      </c>
       <c r="E24" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
     </row>
     <row r="25" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B25" t="s">
+        <v>209</v>
+      </c>
+      <c r="C25" t="s">
         <v>210</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="D25" s="4" t="s">
-        <v>212</v>
-      </c>
       <c r="E25" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>151</v>
+        <v>187</v>
       </c>
       <c r="G25" s="4" t="s">
         <v>40</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B26" t="s">
+        <v>86</v>
+      </c>
+      <c r="C26" t="s">
         <v>87</v>
       </c>
-      <c r="C26" t="s">
-        <v>88</v>
-      </c>
       <c r="D26" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>151</v>
+        <v>187</v>
       </c>
       <c r="G26" s="4" t="s">
         <v>40</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B27" t="s">
+        <v>96</v>
+      </c>
+      <c r="C27" t="s">
         <v>97</v>
       </c>
-      <c r="C27" t="s">
-        <v>98</v>
-      </c>
       <c r="D27" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>151</v>
+        <v>187</v>
       </c>
       <c r="G27" s="4" t="s">
         <v>40</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B28" t="s">
+        <v>98</v>
+      </c>
+      <c r="C28" t="s">
         <v>99</v>
       </c>
-      <c r="C28" t="s">
-        <v>100</v>
-      </c>
       <c r="D28" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>151</v>
+        <v>187</v>
       </c>
       <c r="G28" s="4" t="s">
         <v>40</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B29" t="s">
+        <v>212</v>
+      </c>
+      <c r="C29" t="s">
         <v>213</v>
       </c>
-      <c r="C29" t="s">
-        <v>214</v>
-      </c>
       <c r="D29" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>151</v>
+        <v>187</v>
       </c>
       <c r="G29" s="4" t="s">
         <v>40</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B30" t="s">
+        <v>73</v>
+      </c>
+      <c r="C30" t="s">
         <v>74</v>
       </c>
-      <c r="C30" t="s">
-        <v>75</v>
-      </c>
       <c r="D30" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>151</v>
+        <v>187</v>
       </c>
       <c r="G30" s="4" t="s">
         <v>40</v>
@@ -1927,22 +1927,22 @@
     </row>
     <row r="31" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B31" t="s">
+        <v>75</v>
+      </c>
+      <c r="C31" t="s">
         <v>76</v>
       </c>
-      <c r="C31" t="s">
-        <v>77</v>
-      </c>
       <c r="D31" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>151</v>
+        <v>187</v>
       </c>
       <c r="G31" s="4" t="s">
         <v>41</v>
@@ -1953,22 +1953,22 @@
     </row>
     <row r="32" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B32" t="s">
+        <v>77</v>
+      </c>
+      <c r="C32" t="s">
         <v>78</v>
       </c>
-      <c r="C32" t="s">
-        <v>79</v>
-      </c>
       <c r="D32" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>151</v>
+        <v>187</v>
       </c>
       <c r="G32" s="4" t="s">
         <v>42</v>
@@ -1979,22 +1979,22 @@
     </row>
     <row r="33" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B33" t="s">
+        <v>79</v>
+      </c>
+      <c r="C33" t="s">
         <v>80</v>
       </c>
-      <c r="C33" t="s">
-        <v>81</v>
-      </c>
       <c r="D33" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>151</v>
+        <v>187</v>
       </c>
       <c r="G33" s="4" t="s">
         <v>40</v>
@@ -2005,22 +2005,22 @@
     </row>
     <row r="34" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B34" t="s">
+        <v>81</v>
+      </c>
+      <c r="C34" t="s">
         <v>82</v>
       </c>
-      <c r="C34" t="s">
-        <v>83</v>
-      </c>
       <c r="D34" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>151</v>
+        <v>187</v>
       </c>
       <c r="G34" s="4" t="s">
         <v>40</v>
@@ -2031,22 +2031,22 @@
     </row>
     <row r="35" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B35" t="s">
+        <v>83</v>
+      </c>
+      <c r="C35" t="s">
         <v>84</v>
       </c>
-      <c r="C35" t="s">
-        <v>85</v>
-      </c>
       <c r="D35" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>151</v>
+        <v>187</v>
       </c>
       <c r="G35" s="4" t="s">
         <v>40</v>
@@ -2057,22 +2057,22 @@
     </row>
     <row r="36" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B36" t="s">
+        <v>113</v>
+      </c>
+      <c r="C36" t="s">
         <v>114</v>
       </c>
-      <c r="C36" t="s">
-        <v>115</v>
-      </c>
       <c r="D36" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E36" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="F36" s="2" t="s">
         <v>150</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>151</v>
       </c>
       <c r="G36" s="4" t="s">
         <v>34</v>
@@ -2083,22 +2083,22 @@
     </row>
     <row r="37" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B37" t="s">
+        <v>115</v>
+      </c>
+      <c r="C37" t="s">
         <v>116</v>
       </c>
-      <c r="C37" t="s">
+      <c r="D37" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="D37" s="4" t="s">
-        <v>118</v>
-      </c>
       <c r="E37" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="F37" s="2" t="s">
         <v>150</v>
-      </c>
-      <c r="F37" s="2" t="s">
-        <v>151</v>
       </c>
       <c r="G37" s="4" t="s">
         <v>34</v>
@@ -2109,22 +2109,22 @@
     </row>
     <row r="38" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B38" t="s">
+        <v>184</v>
+      </c>
+      <c r="C38" t="s">
         <v>185</v>
       </c>
-      <c r="C38" t="s">
+      <c r="D38" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="D38" s="4" t="s">
-        <v>187</v>
-      </c>
       <c r="E38" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G38" s="4" t="s">
         <v>43</v>
@@ -2135,22 +2135,22 @@
     </row>
     <row r="39" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B39" t="s">
+        <v>188</v>
+      </c>
+      <c r="C39" t="s">
         <v>189</v>
       </c>
-      <c r="C39" t="s">
+      <c r="D39" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="D39" s="4" t="s">
-        <v>191</v>
-      </c>
       <c r="E39" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G39" s="4" t="s">
         <v>44</v>
@@ -2161,22 +2161,22 @@
     </row>
     <row r="40" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B40" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C40" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G40" s="4" t="s">
         <v>34</v>
@@ -2187,22 +2187,22 @@
     </row>
     <row r="41" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B41" t="s">
+        <v>193</v>
+      </c>
+      <c r="C41" t="s">
         <v>194</v>
       </c>
-      <c r="C41" t="s">
-        <v>195</v>
-      </c>
       <c r="D41" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>151</v>
+        <v>187</v>
       </c>
       <c r="G41" s="4" t="s">
         <v>34</v>
@@ -2213,22 +2213,22 @@
     </row>
     <row r="42" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B42" t="s">
+        <v>195</v>
+      </c>
+      <c r="C42" t="s">
         <v>196</v>
       </c>
-      <c r="C42" t="s">
-        <v>197</v>
-      </c>
       <c r="D42" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E42" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="F42" s="1" t="s">
         <v>150</v>
-      </c>
-      <c r="F42" s="1" t="s">
-        <v>151</v>
       </c>
       <c r="G42" s="4" t="s">
         <v>34</v>
@@ -2239,22 +2239,22 @@
     </row>
     <row r="43" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B43" t="s">
+        <v>197</v>
+      </c>
+      <c r="C43" t="s">
         <v>198</v>
       </c>
-      <c r="C43" t="s">
-        <v>199</v>
-      </c>
       <c r="D43" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>151</v>
+        <v>187</v>
       </c>
       <c r="G43" s="4" t="s">
         <v>34</v>
@@ -2265,22 +2265,22 @@
     </row>
     <row r="44" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B44" t="s">
+        <v>199</v>
+      </c>
+      <c r="C44" t="s">
         <v>200</v>
       </c>
-      <c r="C44" t="s">
-        <v>201</v>
-      </c>
       <c r="D44" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E44" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="F44" s="1" t="s">
         <v>150</v>
-      </c>
-      <c r="F44" s="1" t="s">
-        <v>151</v>
       </c>
       <c r="G44" s="4" t="s">
         <v>34</v>
@@ -2291,22 +2291,22 @@
     </row>
     <row r="45" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C45" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D45" s="6">
         <v>0.13194444444444445</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G45" s="2" t="s">
         <v>15</v>
@@ -2317,22 +2317,22 @@
     </row>
     <row r="46" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="B46" t="s">
+        <v>126</v>
+      </c>
+      <c r="C46" t="s">
         <v>125</v>
-      </c>
-      <c r="B46" t="s">
-        <v>127</v>
-      </c>
-      <c r="C46" t="s">
-        <v>126</v>
       </c>
       <c r="D46" s="6">
         <v>0.2388888888888889</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G46" s="2" t="s">
         <v>15</v>
@@ -2343,22 +2343,22 @@
     </row>
     <row r="47" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C47" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D47" s="6">
         <v>0.12291666666666667</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G47" s="2" t="s">
         <v>15</v>
@@ -2369,22 +2369,22 @@
     </row>
     <row r="48" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C48" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D48" s="6">
         <v>0.13333333333333333</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G48" s="2" t="s">
         <v>15</v>
@@ -2395,22 +2395,22 @@
     </row>
     <row r="49" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B49" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C49" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G49" s="2" t="s">
         <v>15</v>
@@ -2421,22 +2421,22 @@
     </row>
     <row r="50" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B50" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C50" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D50" t="s">
+        <v>118</v>
+      </c>
+      <c r="E50" t="s">
         <v>119</v>
       </c>
-      <c r="E50" t="s">
-        <v>120</v>
-      </c>
       <c r="F50" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G50" s="2" t="s">
         <v>16</v>
@@ -2447,22 +2447,22 @@
     </row>
     <row r="51" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B51" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C51" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D51" t="s">
+        <v>120</v>
+      </c>
+      <c r="E51" t="s">
         <v>121</v>
       </c>
-      <c r="E51" t="s">
-        <v>122</v>
-      </c>
       <c r="F51" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G51" s="2" t="s">
         <v>16</v>
@@ -2473,22 +2473,22 @@
     </row>
     <row r="52" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B52" t="s">
+        <v>107</v>
+      </c>
+      <c r="C52" t="s">
+        <v>207</v>
+      </c>
+      <c r="D52" t="s">
+        <v>109</v>
+      </c>
+      <c r="E52" t="s">
         <v>108</v>
       </c>
-      <c r="C52" t="s">
-        <v>208</v>
-      </c>
-      <c r="D52" t="s">
-        <v>110</v>
-      </c>
-      <c r="E52" t="s">
-        <v>109</v>
-      </c>
       <c r="F52" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G52" s="2" t="s">
         <v>16</v>
@@ -2499,22 +2499,22 @@
     </row>
     <row r="53" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B53" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C53" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D53" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E53" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G53" s="2" t="s">
         <v>15</v>
@@ -2525,22 +2525,22 @@
     </row>
     <row r="54" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B54" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C54" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D54" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E54" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G54" s="2" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
All art done, asset list updated.
</commit_message>
<xml_diff>
--- a/Doorman_Documents/Asset List.xlsx
+++ b/Doorman_Documents/Asset List.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="230">
   <si>
     <t>flour</t>
     <phoneticPr fontId="4" type="noConversion"/>
@@ -168,10 +168,6 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>Placeholder</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>bg</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
@@ -548,9 +544,6 @@
     <t>Image by Kyle</t>
   </si>
   <si>
-    <t>Placeholder</t>
-  </si>
-  <si>
     <t>File Name</t>
   </si>
   <si>
@@ -777,6 +770,21 @@
   </si>
   <si>
     <t>Bg_City.jpg</t>
+  </si>
+  <si>
+    <t>Item_Notebook.png</t>
+  </si>
+  <si>
+    <t>966 X 1080</t>
+  </si>
+  <si>
+    <t>Item_Notebookicon.png</t>
+  </si>
+  <si>
+    <t>Clickable icon that opens notebook</t>
+  </si>
+  <si>
+    <t>Notebook with list of what info you need to be able to steal</t>
   </si>
 </sst>
 </file>
@@ -1126,44 +1134,44 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0"/>
-  <dimension ref="A1:AC71"/>
+  <dimension ref="A1:AC73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.109375" customWidth="1"/>
     <col min="2" max="2" width="32.33203125" customWidth="1"/>
-    <col min="3" max="3" width="43.6640625" customWidth="1"/>
+    <col min="3" max="3" width="50.21875" customWidth="1"/>
     <col min="5" max="5" width="57" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>141</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>142</v>
       </c>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
@@ -1189,1397 +1197,1435 @@
     </row>
     <row r="2" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>214</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>215</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>216</v>
-      </c>
       <c r="E3" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
     </row>
     <row r="4" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B4" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C4" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B5" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C5" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="B6" t="s">
         <v>143</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
+        <v>156</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="G6" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="C6" t="s">
-        <v>158</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>145</v>
-      </c>
       <c r="H6" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B7" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C7" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B8" t="s">
+        <v>215</v>
+      </c>
+      <c r="C8" t="s">
+        <v>216</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>217</v>
       </c>
-      <c r="C8" t="s">
-        <v>218</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>219</v>
-      </c>
       <c r="E8" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
     </row>
     <row r="9" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B9" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C9" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
     </row>
     <row r="10" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B10" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C10" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B11" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C11" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="B12" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="C12" s="8" t="s">
         <v>135</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>136</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>35</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>35</v>
       </c>
       <c r="E13" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="H13" s="4" t="s">
         <v>54</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B14" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C14" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B15" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C15" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B16" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>35</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F16" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="G16" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="G16" s="4" t="s">
-        <v>37</v>
-      </c>
       <c r="H16" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B17" t="s">
+        <v>167</v>
+      </c>
+      <c r="C17" t="s">
+        <v>168</v>
+      </c>
+      <c r="D17" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="C17" t="s">
-        <v>170</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>171</v>
-      </c>
       <c r="E17" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B18" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C18" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B19" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C19" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B20" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C20" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B21" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C21" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B22" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C22" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B23" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C23" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B24" t="s">
+        <v>220</v>
+      </c>
+      <c r="C24" t="s">
+        <v>221</v>
+      </c>
+      <c r="D24" s="4" t="s">
         <v>222</v>
       </c>
-      <c r="C24" t="s">
-        <v>223</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>224</v>
-      </c>
       <c r="E24" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
     </row>
     <row r="25" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B25" t="s">
+        <v>207</v>
+      </c>
+      <c r="C25" t="s">
+        <v>208</v>
+      </c>
+      <c r="D25" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="C25" t="s">
-        <v>210</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>211</v>
-      </c>
       <c r="E25" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B26" t="s">
+        <v>85</v>
+      </c>
+      <c r="C26" t="s">
         <v>86</v>
       </c>
-      <c r="C26" t="s">
-        <v>87</v>
-      </c>
       <c r="D26" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B27" t="s">
+        <v>95</v>
+      </c>
+      <c r="C27" t="s">
         <v>96</v>
       </c>
-      <c r="C27" t="s">
-        <v>97</v>
-      </c>
       <c r="D27" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B28" t="s">
+        <v>97</v>
+      </c>
+      <c r="C28" t="s">
         <v>98</v>
       </c>
-      <c r="C28" t="s">
-        <v>99</v>
-      </c>
       <c r="D28" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B29" t="s">
-        <v>212</v>
+        <v>225</v>
       </c>
       <c r="C29" t="s">
-        <v>213</v>
+        <v>229</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>88</v>
+        <v>226</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="G29" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="H29" s="4" t="s">
-        <v>69</v>
-      </c>
+        <v>185</v>
+      </c>
+      <c r="G29" s="4"/>
+      <c r="H29" s="4"/>
     </row>
     <row r="30" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B30" t="s">
-        <v>73</v>
+        <v>227</v>
       </c>
       <c r="C30" t="s">
-        <v>74</v>
+        <v>228</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="G30" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="H30" s="4" t="s">
-        <v>0</v>
-      </c>
+        <v>185</v>
+      </c>
+      <c r="G30" s="4"/>
+      <c r="H30" s="4"/>
     </row>
     <row r="31" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B31" t="s">
-        <v>75</v>
+        <v>210</v>
       </c>
       <c r="C31" t="s">
-        <v>76</v>
+        <v>211</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H31" s="4" t="s">
-        <v>1</v>
+        <v>68</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B32" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C32" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="H32" s="4" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B33" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C33" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="G33" s="4" t="s">
         <v>40</v>
       </c>
       <c r="H33" s="4" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B34" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C34" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H34" s="4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B35" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C35" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B36" t="s">
-        <v>113</v>
+        <v>80</v>
       </c>
       <c r="C36" t="s">
-        <v>114</v>
+        <v>81</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>117</v>
+        <v>92</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>150</v>
+        <v>185</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="H36" s="4" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B37" t="s">
+        <v>82</v>
+      </c>
+      <c r="C37" t="s">
+        <v>83</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="G37" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="H37" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="B38" t="s">
+        <v>112</v>
+      </c>
+      <c r="C38" t="s">
+        <v>113</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="G38" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H38" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="B39" t="s">
+        <v>114</v>
+      </c>
+      <c r="C39" t="s">
         <v>115</v>
       </c>
-      <c r="C37" t="s">
+      <c r="D39" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="D37" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="E37" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="F37" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="G37" s="4" t="s">
+      <c r="E39" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="G39" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="H37" s="4" t="s">
+      <c r="H39" s="4" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A38" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="B38" t="s">
-        <v>184</v>
-      </c>
-      <c r="C38" t="s">
-        <v>185</v>
-      </c>
-      <c r="D38" s="4" t="s">
-        <v>186</v>
-      </c>
-      <c r="E38" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="G38" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="H38" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A39" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="B39" t="s">
-        <v>188</v>
-      </c>
-      <c r="C39" t="s">
-        <v>189</v>
-      </c>
-      <c r="D39" s="4" t="s">
-        <v>190</v>
-      </c>
-      <c r="E39" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="G39" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="H39" s="4" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B40" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="C40" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>148</v>
+        <v>184</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="G40" s="4" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="H40" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B41" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="C41" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>148</v>
+        <v>188</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>100</v>
+        <v>148</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="G41" s="4" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="H41" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B42" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="C42" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>150</v>
+        <v>185</v>
       </c>
       <c r="G42" s="4" t="s">
         <v>34</v>
       </c>
       <c r="H42" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B43" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="C43" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="G43" s="4" t="s">
         <v>34</v>
       </c>
       <c r="H43" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B44" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="C44" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>150</v>
+        <v>185</v>
       </c>
       <c r="G44" s="4" t="s">
         <v>34</v>
       </c>
       <c r="H44" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="B45" s="7" t="s">
-        <v>131</v>
+        <v>142</v>
+      </c>
+      <c r="B45" t="s">
+        <v>195</v>
       </c>
       <c r="C45" t="s">
-        <v>201</v>
-      </c>
-      <c r="D45" s="6">
-        <v>0.13194444444444445</v>
-      </c>
-      <c r="E45" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="F45" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="G45" s="2" t="s">
-        <v>15</v>
+        <v>196</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="G45" s="4" t="s">
+        <v>34</v>
       </c>
       <c r="H45" s="4" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
-        <v>124</v>
+        <v>142</v>
       </c>
       <c r="B46" t="s">
-        <v>126</v>
+        <v>197</v>
       </c>
       <c r="C46" t="s">
-        <v>125</v>
-      </c>
-      <c r="D46" s="6">
-        <v>0.2388888888888889</v>
-      </c>
-      <c r="E46" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="F46" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="G46" s="2" t="s">
-        <v>15</v>
+        <v>198</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="E46" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="G46" s="4" t="s">
+        <v>34</v>
       </c>
       <c r="H46" s="4" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
     </row>
     <row r="47" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B47" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="C47" t="s">
+        <v>199</v>
+      </c>
+      <c r="D47" s="6">
+        <v>0.13194444444444445</v>
+      </c>
+      <c r="E47" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="C47" t="s">
-        <v>202</v>
-      </c>
-      <c r="D47" s="6">
-        <v>0.12291666666666667</v>
-      </c>
-      <c r="E47" s="5" t="s">
-        <v>128</v>
-      </c>
       <c r="F47" s="2" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="G47" s="2" t="s">
         <v>15</v>
       </c>
       <c r="H47" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="B48" t="s">
+        <v>125</v>
+      </c>
+      <c r="C48" t="s">
         <v>124</v>
       </c>
-      <c r="B48" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="C48" t="s">
-        <v>203</v>
-      </c>
       <c r="D48" s="6">
-        <v>0.13333333333333333</v>
+        <v>0.2388888888888889</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="G48" s="2" t="s">
         <v>15</v>
       </c>
       <c r="H48" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="49" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="B49" t="s">
-        <v>101</v>
+        <v>123</v>
+      </c>
+      <c r="B49" s="7" t="s">
+        <v>128</v>
       </c>
       <c r="C49" t="s">
-        <v>204</v>
-      </c>
-      <c r="D49" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="E49" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="F49" s="1" t="s">
-        <v>225</v>
+        <v>200</v>
+      </c>
+      <c r="D49" s="6">
+        <v>0.12291666666666667</v>
+      </c>
+      <c r="E49" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>223</v>
       </c>
       <c r="G49" s="2" t="s">
         <v>15</v>
       </c>
       <c r="H49" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="50" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="B50" t="s">
-        <v>122</v>
+        <v>123</v>
+      </c>
+      <c r="B50" s="7" t="s">
+        <v>132</v>
       </c>
       <c r="C50" t="s">
-        <v>205</v>
-      </c>
-      <c r="D50" t="s">
-        <v>118</v>
-      </c>
-      <c r="E50" t="s">
-        <v>119</v>
-      </c>
-      <c r="F50" s="1" t="s">
-        <v>225</v>
+        <v>201</v>
+      </c>
+      <c r="D50" s="6">
+        <v>0.13333333333333333</v>
+      </c>
+      <c r="E50" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>223</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H50" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="51" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B51" t="s">
-        <v>123</v>
+        <v>100</v>
       </c>
       <c r="C51" t="s">
-        <v>206</v>
-      </c>
-      <c r="D51" t="s">
-        <v>120</v>
-      </c>
-      <c r="E51" t="s">
-        <v>121</v>
+        <v>202</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="E51" s="4" t="s">
+        <v>102</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H51" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="52" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B52" t="s">
-        <v>107</v>
+        <v>121</v>
       </c>
       <c r="C52" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="D52" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="E52" t="s">
-        <v>108</v>
+        <v>118</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="G52" s="2" t="s">
         <v>16</v>
       </c>
       <c r="H52" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="53" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B53" t="s">
-        <v>105</v>
+        <v>122</v>
       </c>
       <c r="C53" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D53" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
       <c r="E53" t="s">
-        <v>104</v>
+        <v>120</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="G53" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H53" s="8" t="s">
-        <v>25</v>
+        <v>16</v>
+      </c>
+      <c r="H53" s="4" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="54" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B54" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="C54" t="s">
-        <v>85</v>
+        <v>205</v>
       </c>
       <c r="D54" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E54" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="G54" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H54" s="8" t="s">
-        <v>24</v>
+      <c r="H54" s="4" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="55" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="B55" t="s">
+        <v>104</v>
+      </c>
+      <c r="C55" t="s">
+        <v>206</v>
+      </c>
+      <c r="D55" t="s">
+        <v>109</v>
+      </c>
+      <c r="E55" t="s">
+        <v>103</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="G55" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H55" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A56" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="B56" t="s">
+        <v>101</v>
+      </c>
+      <c r="C56" t="s">
+        <v>84</v>
+      </c>
+      <c r="D56" t="s">
+        <v>110</v>
+      </c>
+      <c r="E56" t="s">
+        <v>105</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="G56" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H56" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A57" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B55" s="8" t="s">
+      <c r="B57" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C55" s="8" t="s">
+      <c r="C57" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D55" s="8" t="s">
+      <c r="D57" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="E55" s="7" t="s">
+      <c r="E57" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="F55" s="2" t="s">
+      <c r="F57" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G55" s="2" t="s">
+      <c r="G57" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H55" t="s">
+      <c r="H57" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="56" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="F56" s="1"/>
-    </row>
-    <row r="57" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="F57" s="1"/>
     </row>
     <row r="58" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="F58" s="1"/>
@@ -2622,6 +2668,12 @@
     </row>
     <row r="71" spans="6:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="F71" s="1"/>
+    </row>
+    <row r="72" spans="6:6" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F72" s="1"/>
+    </row>
+    <row r="73" spans="6:6" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F73" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>

</xml_diff>